<commit_message>
[ADD] My peer review sprint 2
</commit_message>
<xml_diff>
--- a/Team Docs/PeerReview_Rob.xlsx
+++ b/Team Docs/PeerReview_Rob.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project-startup\Team Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CCA7F533-B252-47B8-91D0-C260BC6C4B29}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1009EECC-AB3F-4EF9-93EF-B5AB1BF201C6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Week 2 Review" sheetId="1" r:id="rId1"/>
-    <sheet name="Week 4 Review" sheetId="2" r:id="rId2"/>
-    <sheet name="Week 6 Review" sheetId="3" r:id="rId3"/>
+    <sheet name="Sprint 1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sprint 2" sheetId="6" r:id="rId2"/>
+    <sheet name="Sprint 3" sheetId="3" r:id="rId3"/>
     <sheet name="Progress Overview" sheetId="4" r:id="rId4"/>
     <sheet name="Data" sheetId="5" state="hidden" r:id="rId5"/>
   </sheets>
@@ -24,6 +24,7 @@
     <externalReference r:id="rId7"/>
     <externalReference r:id="rId8"/>
     <externalReference r:id="rId9"/>
+    <externalReference r:id="rId10"/>
   </externalReferences>
   <calcPr calcId="181029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="536" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="546" uniqueCount="115">
   <si>
     <t>PEER1</t>
   </si>
@@ -385,21 +386,59 @@
   </si>
   <si>
     <t>Strength(s):
-You work fast for prototyping with a focus on the priorities. You work with C# with expertise and efficiency. With C++ you don't shy away from challenge despite having mentioned that Engine dev and C++ is daunting. You ask for help when you need it and are willing to lend out a helping hand whenever it is needed. You get done what is needed.
-Improvement(s):
-Your understanding of more advanced C++ concepts can use improvement. If you're stuck with C++ you could ask for help sooner or for tips for research directions.</t>
-  </si>
-  <si>
-    <t>Strength(s):
 Skilled in C++ and engine development. Feels responsible for his tasks. Is willing to put in extra work when necessary. made improvements in trusting other programmers to implement sensitive systems.
 Improvement(s):
 Workload delegation, you could spread out your wokload more between the other programmers. Implementation time underestimation, despite adding 30% more implementation time you still manage to spend more time than the actual estimation. You should trust your fellow programmers more with intricate and complicated core systems. You tend to try to overcomplicate implementations for only a slightly bigger convenience for other team members, ask your temmembers to spend 5 seconds more instead of spending hours more yourself. Don't be a perfectionistic little bitch.</t>
   </si>
   <si>
+    <t xml:space="preserve">As a summary, according to my team mates I always deliever what's asked from me in high quality and can be relied on even in areas that are not my expertise. I always ask for feedback, even during the process.
+</t>
+  </si>
+  <si>
+    <t>For improvments I need to be more communicative with my team mates during work, meaning less time on headphones and more time being present.</t>
+  </si>
+  <si>
+    <t>Received very helpful feedback: Be more confident, grant myself more work time and give more feedback to peers.</t>
+  </si>
+  <si>
+    <t>Give myself more work time, keep asking for feedback about my work, give feedback to others more.</t>
+  </si>
+  <si>
+    <t>Quick at making prototypes and isn't afraid to add or remove features when asked. Gets distracted sometimes. Gives advice but sometimes get stuck on specific points. Learn more about advanced c++ concepts and ask sooner for help.</t>
+  </si>
+  <si>
+    <t>Dabble with more C++ in general but more specifically advanced data structures. Make decisions more quickly instead of arguing about it.</t>
+  </si>
+  <si>
     <t>Strength(s):
-You deliver your work in a timely manner to the best of your abilities. Despite having daunting complicated tasks in an unknown engine and with a failry daunting unknown language you don't shy away from struggling through it anyways and delivering performance.
+You work fast for prototyping with a focus on the priorities. You work with C# with expertise and efficiency. With C++ you don't shy away from challenge despite having mentioned that Engine dev and C++ is daunting. You ask for help when you need it and are willing to lend out a helping hand whenever it is needed. You get done what is needed.
 Improvement(s):
-C++ skills in more advanced topics could be improved. You lack confidence in your code. You are a good programmer, acknowledge that.</t>
+Your understanding of more advanced C++ concepts can use improvement. If you're stuck with C++ you could ask for help sooner or for tips for research directions.
+You should learn more about advanced data structures.</t>
+  </si>
+  <si>
+    <t>Strength(s):
+You deliver your work in a timely manner to the best of your abilities. Despite having daunting complicated tasks in an unknown engine and with a failry daunting unknown language you don't shy away from struggling through it anyways and delivering performance. You add a positive feel to the team.
+Improvement(s):
+C++ skills in more advanced topics could be improved. You lack confidence in your code. You are a good programmer, acknowledge that.
+You can spend more attention on being on time.
+You should learn more about advanced data structures.</t>
+  </si>
+  <si>
+    <t>I keep getting stuck on no longer relevant topics during discussions, dragging out discussions unnecessarily. Should learn better time management.</t>
+  </si>
+  <si>
+    <t>I should rethink whether what I want to say is really still relevant. I should trust my fellow programmers with bigger tasks and add an even higher time margin to tasks.</t>
+  </si>
+  <si>
+    <t>I planned well for the sprint, good a keeping meetings and
+discussions streamlined, I have a good work ethic and
+can improvise</t>
+  </si>
+  <si>
+    <t>I will keep my working hours between 09.30 and 17.00 for 
+most days, I will also try and listen to other peoples ideas 
+a lot better</t>
   </si>
   <si>
     <t xml:space="preserve">Strength(s): Made the initial prototype very quicky
@@ -410,21 +449,341 @@
 </t>
   </si>
   <si>
-    <t>I planned well for the sprint, good a keeping meetings and
-discussions streamlined, I have a good work ethic and
-can improvise</t>
-  </si>
-  <si>
-    <t>I will keep my working hours between 09.30 and 17.00 for 
-most days, I will also try and listen to other peoples ideas 
-a lot better</t>
+    <t xml:space="preserve">
+</t>
+  </si>
+  <si>
+    <t>Strength(s):
+Improvement(s):</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Strength(s):
+Improvement(s): 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Strength(s):
+Improvement(s): 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Strength(s):
+Improvement(s):
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Strength(s):
+Improvement(s):
+</t>
+  </si>
+  <si>
+    <t>Strength(s):
+Improvement(s):</t>
+  </si>
+  <si>
+    <t>Strength(s):
+.
+Improvement(s):
+.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Strength(s):
+.
+Improvement(s):
+</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Strength(s):
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>- Great team management skills, probably the best I've ever experienced.
+- Very flexible, can do almost any role well.
+- Quick to concept and improvise.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">
+Improvement(s):
+- </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Sometimes gets involved in other conversations that aren't related to the project or work. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Strength(s):
+- </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Can make really good art in really quick time.
+- Always asks for advice and feedback.
+- Can separate work from personal life, always has a smile that makes her approachable.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">
+Improvement(s):
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Really can't think of any, stop making cool art it makes the other artists look bad.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Strength(s):
+- </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Good at music and sound in general.
+- Asks for help and feedback.
+- Passionante about what he makes.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+Improvement(s):
+- </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Coming on time can be worked on more.
+- Some tasks take far too long than they should.
+- Doesn't trust his own skills.
+- Should be more communicative.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Strength(s):
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>- Funny and social which makes working with him really fun.
+- Eager to learn new things and develop his own skills.
+- Good programmer and can fix stuff quickly and easily.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">
+Improvement(s):
+- </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Sometimes gets caught up with other things, but I don't see it hindering the progress.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Strength(s):
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>- Great programmer and has a knack for technical thinking.
+- I don't understand programming but I can tell he's a good source of knowledge and he doesn't shy from taking some as well.
+- Very dedicated to work.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">
+Improvement(s):
+- </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Should stop overworking himself and pay attention to other things than work.
+- Sometimes get's overly involved in irrelevant disscussions.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Strength(s):
+-</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Extremely reliable.
+- Puts a lot of effort in completing his task in a high quality.
+- Doesn't shy from going out of his comfort zone.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">
+- </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Always happy and brings up group morale.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">
+Improvement(s):
+- </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>More attention to getting here on time.</t>
+    </r>
+  </si>
+  <si>
+    <t>Strength(s): Was on time most of the again which I was happy with
+Improvement(s): 
+I planned to many hours of tasks for myself this week</t>
+  </si>
+  <si>
+    <t>Strength(s): Really nice 3D art. Great wirk ethic
+Improvement(s): 
+Trust your judgement more you're talented</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Strength(s):  Work completed on time and to high quality
+Improvement(s): 
+Being on time for the Stand-Ups </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Strength(s): Diviing in to topics that are new to you
+Improvement(s): 
+Could be more punctual 
+</t>
+  </si>
+  <si>
+    <t>Strength(s): Keeping the programmers on track well, and working
+very hard, better at using duck tape
+Improvement(s): 
+Still sometimes getting caught up on things and sometimes
+over working</t>
+  </si>
+  <si>
+    <t>Strength(s): 
+Diving in to new topics well, great help with the prototype
+Improvement(s): 
+N/A</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -472,6 +831,11 @@
     </font>
     <font>
       <sz val="9"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -667,7 +1031,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
@@ -799,6 +1163,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -834,7 +1199,391 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="56">
+  <dxfs count="104">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFCCCCCC"/>
+          <bgColor rgb="FFCCCCCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4CCCC"/>
+          <bgColor rgb="FFF4CCCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFCE5CD"/>
+          <bgColor rgb="FFFCE5CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFF2CC"/>
+          <bgColor rgb="FFFFF2CC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD9EAD3"/>
+          <bgColor rgb="FFD9EAD3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD0E0E3"/>
+          <bgColor rgb="FFD0E0E3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFCFE2F3"/>
+          <bgColor rgb="FFCFE2F3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD9D2E9"/>
+          <bgColor rgb="FFD9D2E9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFCCCCCC"/>
+          <bgColor rgb="FFCCCCCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4CCCC"/>
+          <bgColor rgb="FFF4CCCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFCE5CD"/>
+          <bgColor rgb="FFFCE5CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFF2CC"/>
+          <bgColor rgb="FFFFF2CC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD9EAD3"/>
+          <bgColor rgb="FFD9EAD3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD0E0E3"/>
+          <bgColor rgb="FFD0E0E3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFCFE2F3"/>
+          <bgColor rgb="FFCFE2F3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD9D2E9"/>
+          <bgColor rgb="FFD9D2E9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFCCCCCC"/>
+          <bgColor rgb="FFCCCCCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4CCCC"/>
+          <bgColor rgb="FFF4CCCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFCE5CD"/>
+          <bgColor rgb="FFFCE5CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFF2CC"/>
+          <bgColor rgb="FFFFF2CC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD9EAD3"/>
+          <bgColor rgb="FFD9EAD3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD0E0E3"/>
+          <bgColor rgb="FFD0E0E3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFCFE2F3"/>
+          <bgColor rgb="FFCFE2F3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD9D2E9"/>
+          <bgColor rgb="FFD9D2E9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFCCCCCC"/>
+          <bgColor rgb="FFCCCCCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4CCCC"/>
+          <bgColor rgb="FFF4CCCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFCE5CD"/>
+          <bgColor rgb="FFFCE5CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFF2CC"/>
+          <bgColor rgb="FFFFF2CC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD9EAD3"/>
+          <bgColor rgb="FFD9EAD3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD0E0E3"/>
+          <bgColor rgb="FFD0E0E3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFCFE2F3"/>
+          <bgColor rgb="FFCFE2F3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD9D2E9"/>
+          <bgColor rgb="FFD9D2E9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFCCCCCC"/>
+          <bgColor rgb="FFCCCCCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4CCCC"/>
+          <bgColor rgb="FFF4CCCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFCE5CD"/>
+          <bgColor rgb="FFFCE5CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFF2CC"/>
+          <bgColor rgb="FFFFF2CC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD9EAD3"/>
+          <bgColor rgb="FFD9EAD3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD0E0E3"/>
+          <bgColor rgb="FFD0E0E3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFCFE2F3"/>
+          <bgColor rgb="FFCFE2F3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD9D2E9"/>
+          <bgColor rgb="FFD9D2E9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFCCCCCC"/>
+          <bgColor rgb="FFCCCCCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4CCCC"/>
+          <bgColor rgb="FFF4CCCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFCE5CD"/>
+          <bgColor rgb="FFFCE5CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFF2CC"/>
+          <bgColor rgb="FFFFF2CC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD9EAD3"/>
+          <bgColor rgb="FFD9EAD3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD0E0E3"/>
+          <bgColor rgb="FFD0E0E3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFCFE2F3"/>
+          <bgColor rgb="FFCFE2F3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD9D2E9"/>
+          <bgColor rgb="FFD9D2E9"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -1336,6 +2085,27 @@
 </file>
 
 <file path=xl/externalLinks/externalLink4.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Week 2 Review"/>
+      <sheetName val="Week 4 Review"/>
+      <sheetName val="Week 6 Review"/>
+      <sheetName val="Progress Overview"/>
+      <sheetName val="Data"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="3" refreshError="1"/>
+      <sheetData sheetId="4" refreshError="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink5.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
@@ -1651,13 +2421,13 @@
   </sheetPr>
   <dimension ref="A1:Z18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Z8" sqref="Z8"/>
+    <sheetView topLeftCell="A5" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="X5" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.44140625" customWidth="1"/>
+    <col min="1" max="1" width="7.5546875" customWidth="1"/>
     <col min="2" max="2" width="8.109375" customWidth="1"/>
     <col min="3" max="3" width="18.44140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="50.6640625" customWidth="1"/>
@@ -1681,7 +2451,8 @@
     <col min="22" max="22" width="15.6640625" customWidth="1"/>
     <col min="23" max="23" width="5.109375" customWidth="1"/>
     <col min="24" max="24" width="2.6640625" customWidth="1"/>
-    <col min="25" max="26" width="42" customWidth="1"/>
+    <col min="25" max="25" width="42" customWidth="1"/>
+    <col min="26" max="26" width="42.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1692,33 +2463,33 @@
         <v>1</v>
       </c>
       <c r="C1" s="2"/>
-      <c r="D1" s="47" t="s">
+      <c r="D1" s="48" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="48"/>
-      <c r="F1" s="48"/>
-      <c r="G1" s="48"/>
-      <c r="H1" s="48"/>
-      <c r="I1" s="48"/>
-      <c r="J1" s="48"/>
-      <c r="K1" s="48"/>
-      <c r="L1" s="48"/>
-      <c r="M1" s="48"/>
-      <c r="N1" s="48"/>
-      <c r="O1" s="48"/>
-      <c r="P1" s="48"/>
-      <c r="Q1" s="48"/>
-      <c r="R1" s="48"/>
-      <c r="S1" s="48"/>
-      <c r="T1" s="48"/>
-      <c r="U1" s="49"/>
-      <c r="V1" s="56" t="s">
+      <c r="E1" s="49"/>
+      <c r="F1" s="49"/>
+      <c r="G1" s="49"/>
+      <c r="H1" s="49"/>
+      <c r="I1" s="49"/>
+      <c r="J1" s="49"/>
+      <c r="K1" s="49"/>
+      <c r="L1" s="49"/>
+      <c r="M1" s="49"/>
+      <c r="N1" s="49"/>
+      <c r="O1" s="49"/>
+      <c r="P1" s="49"/>
+      <c r="Q1" s="49"/>
+      <c r="R1" s="49"/>
+      <c r="S1" s="49"/>
+      <c r="T1" s="49"/>
+      <c r="U1" s="50"/>
+      <c r="V1" s="57" t="s">
         <v>3</v>
       </c>
-      <c r="W1" s="48"/>
-      <c r="X1" s="48"/>
-      <c r="Y1" s="48"/>
-      <c r="Z1" s="48"/>
+      <c r="W1" s="49"/>
+      <c r="X1" s="49"/>
+      <c r="Y1" s="49"/>
+      <c r="Z1" s="49"/>
     </row>
     <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
@@ -1728,31 +2499,31 @@
         <v>12</v>
       </c>
       <c r="C2" s="5"/>
-      <c r="D2" s="50" t="s">
+      <c r="D2" s="51" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="51"/>
-      <c r="F2" s="51"/>
-      <c r="G2" s="51"/>
-      <c r="H2" s="51"/>
-      <c r="I2" s="51"/>
-      <c r="J2" s="51"/>
-      <c r="K2" s="51"/>
-      <c r="L2" s="51"/>
-      <c r="M2" s="51"/>
-      <c r="N2" s="51"/>
-      <c r="O2" s="51"/>
-      <c r="P2" s="51"/>
-      <c r="Q2" s="51"/>
-      <c r="R2" s="51"/>
-      <c r="S2" s="51"/>
-      <c r="T2" s="51"/>
-      <c r="U2" s="52"/>
-      <c r="V2" s="57"/>
-      <c r="W2" s="51"/>
-      <c r="X2" s="51"/>
-      <c r="Y2" s="51"/>
-      <c r="Z2" s="51"/>
+      <c r="E2" s="52"/>
+      <c r="F2" s="52"/>
+      <c r="G2" s="52"/>
+      <c r="H2" s="52"/>
+      <c r="I2" s="52"/>
+      <c r="J2" s="52"/>
+      <c r="K2" s="52"/>
+      <c r="L2" s="52"/>
+      <c r="M2" s="52"/>
+      <c r="N2" s="52"/>
+      <c r="O2" s="52"/>
+      <c r="P2" s="52"/>
+      <c r="Q2" s="52"/>
+      <c r="R2" s="52"/>
+      <c r="S2" s="52"/>
+      <c r="T2" s="52"/>
+      <c r="U2" s="53"/>
+      <c r="V2" s="58"/>
+      <c r="W2" s="52"/>
+      <c r="X2" s="52"/>
+      <c r="Y2" s="52"/>
+      <c r="Z2" s="52"/>
     </row>
     <row r="3" spans="1:26" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
@@ -1764,31 +2535,31 @@
       <c r="C3" s="41" t="s">
         <v>48</v>
       </c>
-      <c r="D3" s="53" t="s">
+      <c r="D3" s="54" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="54"/>
-      <c r="F3" s="54"/>
-      <c r="G3" s="54"/>
-      <c r="H3" s="54"/>
-      <c r="I3" s="54"/>
-      <c r="J3" s="54"/>
-      <c r="K3" s="54"/>
-      <c r="L3" s="54"/>
-      <c r="M3" s="54"/>
-      <c r="N3" s="54"/>
-      <c r="O3" s="54"/>
-      <c r="P3" s="54"/>
-      <c r="Q3" s="54"/>
-      <c r="R3" s="54"/>
-      <c r="S3" s="54"/>
-      <c r="T3" s="54"/>
-      <c r="U3" s="55"/>
-      <c r="V3" s="58"/>
-      <c r="W3" s="54"/>
-      <c r="X3" s="54"/>
-      <c r="Y3" s="54"/>
-      <c r="Z3" s="54"/>
+      <c r="E3" s="55"/>
+      <c r="F3" s="55"/>
+      <c r="G3" s="55"/>
+      <c r="H3" s="55"/>
+      <c r="I3" s="55"/>
+      <c r="J3" s="55"/>
+      <c r="K3" s="55"/>
+      <c r="L3" s="55"/>
+      <c r="M3" s="55"/>
+      <c r="N3" s="55"/>
+      <c r="O3" s="55"/>
+      <c r="P3" s="55"/>
+      <c r="Q3" s="55"/>
+      <c r="R3" s="55"/>
+      <c r="S3" s="55"/>
+      <c r="T3" s="55"/>
+      <c r="U3" s="56"/>
+      <c r="V3" s="59"/>
+      <c r="W3" s="55"/>
+      <c r="X3" s="55"/>
+      <c r="Y3" s="55"/>
+      <c r="Z3" s="55"/>
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9"/>
@@ -1856,28 +2627,28 @@
       <c r="A5" s="9"/>
       <c r="B5" s="10"/>
       <c r="C5" s="10"/>
-      <c r="D5" s="63" t="s">
+      <c r="D5" s="64" t="s">
         <v>19</v>
       </c>
-      <c r="E5" s="51"/>
-      <c r="F5" s="51"/>
-      <c r="G5" s="51"/>
-      <c r="H5" s="51"/>
-      <c r="I5" s="51"/>
-      <c r="J5" s="51"/>
-      <c r="K5" s="51"/>
-      <c r="L5" s="51"/>
-      <c r="M5" s="51"/>
-      <c r="N5" s="51"/>
-      <c r="O5" s="51"/>
-      <c r="P5" s="51"/>
-      <c r="Q5" s="51"/>
-      <c r="R5" s="51"/>
-      <c r="S5" s="51"/>
-      <c r="T5" s="51"/>
-      <c r="U5" s="51"/>
-      <c r="V5" s="51"/>
-      <c r="W5" s="51"/>
+      <c r="E5" s="52"/>
+      <c r="F5" s="52"/>
+      <c r="G5" s="52"/>
+      <c r="H5" s="52"/>
+      <c r="I5" s="52"/>
+      <c r="J5" s="52"/>
+      <c r="K5" s="52"/>
+      <c r="L5" s="52"/>
+      <c r="M5" s="52"/>
+      <c r="N5" s="52"/>
+      <c r="O5" s="52"/>
+      <c r="P5" s="52"/>
+      <c r="Q5" s="52"/>
+      <c r="R5" s="52"/>
+      <c r="S5" s="52"/>
+      <c r="T5" s="52"/>
+      <c r="U5" s="52"/>
+      <c r="V5" s="52"/>
+      <c r="W5" s="52"/>
       <c r="X5" s="10"/>
       <c r="Y5" s="16" t="s">
         <v>20</v>
@@ -1970,8 +2741,8 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:26" s="46" customFormat="1" ht="100.05" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="62" t="s">
+    <row r="7" spans="1:26" s="46" customFormat="1" ht="100.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="63" t="s">
         <v>26</v>
       </c>
       <c r="B7" s="20">
@@ -1999,7 +2770,7 @@
         <v>8</v>
       </c>
       <c r="J7" s="22" t="s">
-        <v>83</v>
+        <v>93</v>
       </c>
       <c r="K7" s="42">
         <v>8</v>
@@ -2034,14 +2805,14 @@
       <c r="W7" s="24"/>
       <c r="X7" s="25"/>
       <c r="Y7" s="44" t="s">
-        <v>84</v>
+        <v>91</v>
       </c>
       <c r="Z7" s="45" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="8" spans="1:26" ht="100.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="51"/>
+        <v>92</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" s="46" customFormat="1" ht="100.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="52"/>
       <c r="B8" s="20">
         <v>464704</v>
       </c>
@@ -2075,37 +2846,41 @@
       <c r="L8" s="28" t="s">
         <v>57</v>
       </c>
-      <c r="M8" s="29">
+      <c r="M8" s="30">
         <v>7</v>
       </c>
       <c r="N8" s="28" t="s">
         <v>59</v>
       </c>
-      <c r="O8" s="29">
+      <c r="O8" s="30">
         <v>7</v>
       </c>
       <c r="P8" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="Q8" s="29"/>
+      <c r="Q8" s="30"/>
       <c r="R8" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="S8" s="29"/>
+      <c r="S8" s="30"/>
       <c r="T8" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="U8" s="29"/>
+      <c r="U8" s="30"/>
       <c r="V8" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="W8" s="29"/>
+      <c r="W8" s="30"/>
       <c r="X8" s="25"/>
-      <c r="Y8" s="26"/>
-      <c r="Z8" s="27"/>
+      <c r="Y8" s="26" t="s">
+        <v>83</v>
+      </c>
+      <c r="Z8" s="27" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="9" spans="1:26" s="46" customFormat="1" ht="100.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="51"/>
+      <c r="A9" s="52"/>
       <c r="B9" s="20">
         <v>428729</v>
       </c>
@@ -2165,11 +2940,15 @@
       </c>
       <c r="W9" s="24"/>
       <c r="X9" s="25"/>
-      <c r="Y9" s="26"/>
-      <c r="Z9" s="27"/>
+      <c r="Y9" s="26" t="s">
+        <v>81</v>
+      </c>
+      <c r="Z9" s="27" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="10" spans="1:26" s="46" customFormat="1" ht="100.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="51"/>
+      <c r="A10" s="52"/>
       <c r="B10" s="20">
         <v>444711</v>
       </c>
@@ -2229,11 +3008,15 @@
       </c>
       <c r="W10" s="30"/>
       <c r="X10" s="25"/>
-      <c r="Y10" s="26"/>
-      <c r="Z10" s="27"/>
-    </row>
-    <row r="11" spans="1:26" s="46" customFormat="1" ht="100.05" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="51"/>
+      <c r="Y10" s="26" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z10" s="27" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" s="46" customFormat="1" ht="100.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="52"/>
       <c r="B11" s="20">
         <v>445021</v>
       </c>
@@ -2259,19 +3042,19 @@
         <v>8</v>
       </c>
       <c r="J11" s="22" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="K11" s="24">
         <v>8</v>
       </c>
       <c r="L11" s="22" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="M11" s="24">
         <v>7</v>
       </c>
       <c r="N11" s="22" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="O11" s="24">
         <v>8</v>
@@ -2293,11 +3076,15 @@
       </c>
       <c r="W11" s="24"/>
       <c r="X11" s="25"/>
-      <c r="Y11" s="26"/>
-      <c r="Z11" s="27"/>
+      <c r="Y11" s="26" t="s">
+        <v>89</v>
+      </c>
+      <c r="Z11" s="27" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="12" spans="1:26" ht="100.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="51"/>
+      <c r="A12" s="52"/>
       <c r="B12" s="20">
         <v>459575</v>
       </c>
@@ -2349,7 +3136,7 @@
       <c r="Z12" s="27"/>
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="51"/>
+      <c r="A13" s="52"/>
       <c r="B13" s="20">
         <v>12335</v>
       </c>
@@ -2401,7 +3188,7 @@
       <c r="Z13" s="27"/>
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="51"/>
+      <c r="A14" s="52"/>
       <c r="B14" s="20">
         <v>12335</v>
       </c>
@@ -2453,7 +3240,7 @@
       <c r="Z14" s="27"/>
     </row>
     <row r="15" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="51"/>
+      <c r="A15" s="52"/>
       <c r="B15" s="20">
         <v>12335</v>
       </c>
@@ -2505,7 +3292,7 @@
       <c r="Z15" s="27"/>
     </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="51"/>
+      <c r="A16" s="52"/>
       <c r="B16" s="20">
         <v>12335</v>
       </c>
@@ -2635,34 +3422,34 @@
       <c r="Z17" s="32"/>
     </row>
     <row r="18" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="59" t="s">
+      <c r="A18" s="60" t="s">
         <v>40</v>
       </c>
-      <c r="B18" s="60"/>
-      <c r="C18" s="60"/>
-      <c r="D18" s="60"/>
-      <c r="E18" s="60"/>
-      <c r="F18" s="60"/>
-      <c r="G18" s="60"/>
-      <c r="H18" s="60"/>
-      <c r="I18" s="60"/>
-      <c r="J18" s="60"/>
-      <c r="K18" s="60"/>
-      <c r="L18" s="60"/>
-      <c r="M18" s="60"/>
-      <c r="N18" s="60"/>
-      <c r="O18" s="60"/>
-      <c r="P18" s="60"/>
-      <c r="Q18" s="60"/>
-      <c r="R18" s="60"/>
-      <c r="S18" s="60"/>
-      <c r="T18" s="60"/>
-      <c r="U18" s="60"/>
-      <c r="V18" s="60"/>
-      <c r="W18" s="60"/>
-      <c r="X18" s="60"/>
-      <c r="Y18" s="60"/>
-      <c r="Z18" s="61"/>
+      <c r="B18" s="61"/>
+      <c r="C18" s="61"/>
+      <c r="D18" s="61"/>
+      <c r="E18" s="61"/>
+      <c r="F18" s="61"/>
+      <c r="G18" s="61"/>
+      <c r="H18" s="61"/>
+      <c r="I18" s="61"/>
+      <c r="J18" s="61"/>
+      <c r="K18" s="61"/>
+      <c r="L18" s="61"/>
+      <c r="M18" s="61"/>
+      <c r="N18" s="61"/>
+      <c r="O18" s="61"/>
+      <c r="P18" s="61"/>
+      <c r="Q18" s="61"/>
+      <c r="R18" s="61"/>
+      <c r="S18" s="61"/>
+      <c r="T18" s="61"/>
+      <c r="U18" s="61"/>
+      <c r="V18" s="61"/>
+      <c r="W18" s="61"/>
+      <c r="X18" s="61"/>
+      <c r="Y18" s="61"/>
+      <c r="Z18" s="62"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -2674,233 +3461,279 @@
     <mergeCell ref="A7:A16"/>
     <mergeCell ref="D5:W5"/>
   </mergeCells>
-  <conditionalFormatting sqref="E4 G4 I4 K4 M4 O4 Q4 S4 E8 G8 I8 K8 M8 O8 Q8 S8 U17 W17 S12:S17 Q12:Q17 O12:O17 M12:M17 K12:K17 I12:I17 G12:G17 E12:E17">
-    <cfRule type="cellIs" dxfId="55" priority="33" operator="equal">
+  <conditionalFormatting sqref="E4 G4 I4 K4 M4 O4 Q4 S4 U17 W17 S12:S17 Q12:Q17 O12:O17 M12:M17 K12:K17 I12:I17 G12:G17 E12:E17">
+    <cfRule type="cellIs" dxfId="103" priority="81" operator="equal">
       <formula>10</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E4 G4 I4 K4 M4 O4 Q4 S4 E8 G8 I8 K8 M8 O8 Q8 S8 U17 W17 S12:S17 Q12:Q17 O12:O17 M12:M17 K12:K17 I12:I17 G12:G17 E12:E17">
-    <cfRule type="cellIs" dxfId="54" priority="34" operator="between">
+  <conditionalFormatting sqref="E4 G4 I4 K4 M4 O4 Q4 S4 U17 W17 S12:S17 Q12:Q17 O12:O17 M12:M17 K12:K17 I12:I17 G12:G17 E12:E17">
+    <cfRule type="cellIs" dxfId="102" priority="82" operator="between">
       <formula>9.99</formula>
       <formula>9</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E4 G4 I4 K4 M4 O4 Q4 S4 E8 G8 I8 K8 M8 O8 Q8 S8 U17 W17 S12:S17 Q12:Q17 O12:O17 M12:M17 K12:K17 I12:I17 G12:G17 E12:E17">
-    <cfRule type="cellIs" dxfId="53" priority="35" operator="between">
+  <conditionalFormatting sqref="E4 G4 I4 K4 M4 O4 Q4 S4 U17 W17 S12:S17 Q12:Q17 O12:O17 M12:M17 K12:K17 I12:I17 G12:G17 E12:E17">
+    <cfRule type="cellIs" dxfId="101" priority="83" operator="between">
       <formula>8.99</formula>
       <formula>8</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E4 G4 I4 K4 M4 O4 Q4 S4 E8 G8 I8 K8 M8 O8 Q8 S8 U17 W17 S12:S17 Q12:Q17 O12:O17 M12:M17 K12:K17 I12:I17 G12:G17 E12:E17">
-    <cfRule type="cellIs" dxfId="52" priority="36" operator="between">
+  <conditionalFormatting sqref="E4 G4 I4 K4 M4 O4 Q4 S4 U17 W17 S12:S17 Q12:Q17 O12:O17 M12:M17 K12:K17 I12:I17 G12:G17 E12:E17">
+    <cfRule type="cellIs" dxfId="100" priority="84" operator="between">
       <formula>7.99</formula>
       <formula>7</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E4 G4 I4 K4 M4 O4 Q4 S4 E8 G8 I8 K8 M8 O8 Q8 S8 U17 W17 S12:S17 Q12:Q17 O12:O17 M12:M17 K12:K17 I12:I17 G12:G17 E12:E17">
-    <cfRule type="cellIs" dxfId="51" priority="37" operator="between">
+  <conditionalFormatting sqref="E4 G4 I4 K4 M4 O4 Q4 S4 U17 W17 S12:S17 Q12:Q17 O12:O17 M12:M17 K12:K17 I12:I17 G12:G17 E12:E17">
+    <cfRule type="cellIs" dxfId="99" priority="85" operator="between">
       <formula>6.99</formula>
       <formula>6</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E4 G4 I4 K4 M4 O4 Q4 S4 E8 G8 I8 K8 M8 O8 Q8 S8 U17 W17 S12:S17 Q12:Q17 O12:O17 M12:M17 K12:K17 I12:I17 G12:G17 E12:E17">
-    <cfRule type="cellIs" dxfId="50" priority="38" operator="between">
+  <conditionalFormatting sqref="E4 G4 I4 K4 M4 O4 Q4 S4 U17 W17 S12:S17 Q12:Q17 O12:O17 M12:M17 K12:K17 I12:I17 G12:G17 E12:E17">
+    <cfRule type="cellIs" dxfId="98" priority="86" operator="between">
       <formula>5.99</formula>
       <formula>5.5</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E4 G4 I4 K4 M4 O4 Q4 S4 E8 G8 I8 K8 M8 O8 Q8 S8 U17 W17 S12:S17 Q12:Q17 O12:O17 M12:M17 K12:K17 I12:I17 G12:G17 E12:E17">
-    <cfRule type="cellIs" dxfId="49" priority="39" operator="between">
+  <conditionalFormatting sqref="E4 G4 I4 K4 M4 O4 Q4 S4 U17 W17 S12:S17 Q12:Q17 O12:O17 M12:M17 K12:K17 I12:I17 G12:G17 E12:E17">
+    <cfRule type="cellIs" dxfId="97" priority="87" operator="between">
       <formula>5.49</formula>
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E4 G4 I4 K4 M4 O4 Q4 S4 E8 G8 I8 K8 M8 O8 Q8 S8 U17 W17 S12:S17 Q12:Q17 O12:O17 M12:M17 K12:K17 I12:I17 G12:G17 E12:E17">
-    <cfRule type="cellIs" dxfId="48" priority="40" operator="equal">
+  <conditionalFormatting sqref="E4 G4 I4 K4 M4 O4 Q4 S4 U17 W17 S12:S17 Q12:Q17 O12:O17 M12:M17 K12:K17 I12:I17 G12:G17 E12:E17">
+    <cfRule type="cellIs" dxfId="96" priority="88" operator="equal">
       <formula>"NA"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E10 G10 I10 K10 M10 O10 Q10 S10">
-    <cfRule type="cellIs" dxfId="47" priority="25" operator="equal">
+  <conditionalFormatting sqref="E9 G9 I9 K9 M9 O9 Q9 S9">
+    <cfRule type="cellIs" dxfId="95" priority="33" operator="equal">
       <formula>10</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E10 G10 I10 K10 M10 O10 Q10 S10">
-    <cfRule type="cellIs" dxfId="46" priority="26" operator="between">
+  <conditionalFormatting sqref="E9 G9 I9 K9 M9 O9 Q9 S9">
+    <cfRule type="cellIs" dxfId="94" priority="34" operator="between">
       <formula>9.99</formula>
       <formula>9</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E10 G10 I10 K10 M10 O10 Q10 S10">
-    <cfRule type="cellIs" dxfId="45" priority="27" operator="between">
+  <conditionalFormatting sqref="E9 G9 I9 K9 M9 O9 Q9 S9">
+    <cfRule type="cellIs" dxfId="93" priority="35" operator="between">
       <formula>8.99</formula>
       <formula>8</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E10 G10 I10 K10 M10 O10 Q10 S10">
-    <cfRule type="cellIs" dxfId="44" priority="28" operator="between">
+  <conditionalFormatting sqref="E9 G9 I9 K9 M9 O9 Q9 S9">
+    <cfRule type="cellIs" dxfId="92" priority="36" operator="between">
       <formula>7.99</formula>
       <formula>7</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E10 G10 I10 K10 M10 O10 Q10 S10">
-    <cfRule type="cellIs" dxfId="43" priority="29" operator="between">
+  <conditionalFormatting sqref="E9 G9 I9 K9 M9 O9 Q9 S9">
+    <cfRule type="cellIs" dxfId="91" priority="37" operator="between">
       <formula>6.99</formula>
       <formula>6</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E10 G10 I10 K10 M10 O10 Q10 S10">
-    <cfRule type="cellIs" dxfId="42" priority="30" operator="between">
+  <conditionalFormatting sqref="E9 G9 I9 K9 M9 O9 Q9 S9">
+    <cfRule type="cellIs" dxfId="90" priority="38" operator="between">
       <formula>5.99</formula>
       <formula>5.5</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E10 G10 I10 K10 M10 O10 Q10 S10">
-    <cfRule type="cellIs" dxfId="41" priority="31" operator="between">
+  <conditionalFormatting sqref="E9 G9 I9 K9 M9 O9 Q9 S9">
+    <cfRule type="cellIs" dxfId="89" priority="39" operator="between">
       <formula>5.49</formula>
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E10 G10 I10 K10 M10 O10 Q10 S10">
-    <cfRule type="cellIs" dxfId="40" priority="32" operator="equal">
+  <conditionalFormatting sqref="E9 G9 I9 K9 M9 O9 Q9 S9">
+    <cfRule type="cellIs" dxfId="88" priority="40" operator="equal">
       <formula>"NA"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E7 G7 I7 K7 M7 O7 Q7 S7">
-    <cfRule type="cellIs" dxfId="39" priority="17" operator="equal">
+  <conditionalFormatting sqref="E8 G8 I8 K8 M8 O8 Q8 S8">
+    <cfRule type="cellIs" dxfId="87" priority="25" operator="equal">
       <formula>10</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E7 G7 I7 K7 M7 O7 Q7 S7">
-    <cfRule type="cellIs" dxfId="38" priority="18" operator="between">
+  <conditionalFormatting sqref="E8 G8 I8 K8 M8 O8 Q8 S8">
+    <cfRule type="cellIs" dxfId="86" priority="26" operator="between">
       <formula>9.99</formula>
       <formula>9</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E7 G7 I7 K7 M7 O7 Q7 S7">
-    <cfRule type="cellIs" dxfId="37" priority="19" operator="between">
+  <conditionalFormatting sqref="E8 G8 I8 K8 M8 O8 Q8 S8">
+    <cfRule type="cellIs" dxfId="85" priority="27" operator="between">
       <formula>8.99</formula>
       <formula>8</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E7 G7 I7 K7 M7 O7 Q7 S7">
-    <cfRule type="cellIs" dxfId="36" priority="20" operator="between">
+  <conditionalFormatting sqref="E8 G8 I8 K8 M8 O8 Q8 S8">
+    <cfRule type="cellIs" dxfId="84" priority="28" operator="between">
       <formula>7.99</formula>
       <formula>7</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E7 G7 I7 K7 M7 O7 Q7 S7">
-    <cfRule type="cellIs" dxfId="35" priority="21" operator="between">
+  <conditionalFormatting sqref="E8 G8 I8 K8 M8 O8 Q8 S8">
+    <cfRule type="cellIs" dxfId="83" priority="29" operator="between">
       <formula>6.99</formula>
       <formula>6</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E7 G7 I7 K7 M7 O7 Q7 S7">
-    <cfRule type="cellIs" dxfId="34" priority="22" operator="between">
+  <conditionalFormatting sqref="E8 G8 I8 K8 M8 O8 Q8 S8">
+    <cfRule type="cellIs" dxfId="82" priority="30" operator="between">
       <formula>5.99</formula>
       <formula>5.5</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E7 G7 I7 K7 M7 O7 Q7 S7">
-    <cfRule type="cellIs" dxfId="33" priority="23" operator="between">
+  <conditionalFormatting sqref="E8 G8 I8 K8 M8 O8 Q8 S8">
+    <cfRule type="cellIs" dxfId="81" priority="31" operator="between">
       <formula>5.49</formula>
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E7 G7 I7 K7 M7 O7 Q7 S7">
-    <cfRule type="cellIs" dxfId="32" priority="24" operator="equal">
+  <conditionalFormatting sqref="E8 G8 I8 K8 M8 O8 Q8 S8">
+    <cfRule type="cellIs" dxfId="80" priority="32" operator="equal">
       <formula>"NA"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E9 G9 I9 K9 M9 O9 Q9 S9">
-    <cfRule type="cellIs" dxfId="31" priority="9" operator="equal">
+  <conditionalFormatting sqref="E10 G10 I10 K10 M10 O10 Q10 S10">
+    <cfRule type="cellIs" dxfId="79" priority="17" operator="equal">
       <formula>10</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E9 G9 I9 K9 M9 O9 Q9 S9">
-    <cfRule type="cellIs" dxfId="30" priority="10" operator="between">
+  <conditionalFormatting sqref="E10 G10 I10 K10 M10 O10 Q10 S10">
+    <cfRule type="cellIs" dxfId="78" priority="18" operator="between">
       <formula>9.99</formula>
       <formula>9</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E9 G9 I9 K9 M9 O9 Q9 S9">
-    <cfRule type="cellIs" dxfId="29" priority="11" operator="between">
+  <conditionalFormatting sqref="E10 G10 I10 K10 M10 O10 Q10 S10">
+    <cfRule type="cellIs" dxfId="77" priority="19" operator="between">
       <formula>8.99</formula>
       <formula>8</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E9 G9 I9 K9 M9 O9 Q9 S9">
-    <cfRule type="cellIs" dxfId="28" priority="12" operator="between">
+  <conditionalFormatting sqref="E10 G10 I10 K10 M10 O10 Q10 S10">
+    <cfRule type="cellIs" dxfId="76" priority="20" operator="between">
       <formula>7.99</formula>
       <formula>7</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E9 G9 I9 K9 M9 O9 Q9 S9">
-    <cfRule type="cellIs" dxfId="27" priority="13" operator="between">
+  <conditionalFormatting sqref="E10 G10 I10 K10 M10 O10 Q10 S10">
+    <cfRule type="cellIs" dxfId="75" priority="21" operator="between">
       <formula>6.99</formula>
       <formula>6</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E9 G9 I9 K9 M9 O9 Q9 S9">
-    <cfRule type="cellIs" dxfId="26" priority="14" operator="between">
+  <conditionalFormatting sqref="E10 G10 I10 K10 M10 O10 Q10 S10">
+    <cfRule type="cellIs" dxfId="74" priority="22" operator="between">
       <formula>5.99</formula>
       <formula>5.5</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E9 G9 I9 K9 M9 O9 Q9 S9">
-    <cfRule type="cellIs" dxfId="25" priority="15" operator="between">
+  <conditionalFormatting sqref="E10 G10 I10 K10 M10 O10 Q10 S10">
+    <cfRule type="cellIs" dxfId="73" priority="23" operator="between">
       <formula>5.49</formula>
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E9 G9 I9 K9 M9 O9 Q9 S9">
-    <cfRule type="cellIs" dxfId="24" priority="16" operator="equal">
+  <conditionalFormatting sqref="E10 G10 I10 K10 M10 O10 Q10 S10">
+    <cfRule type="cellIs" dxfId="72" priority="24" operator="equal">
       <formula>"NA"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E11 G11 I11 K11 M11 O11 Q11 S11">
-    <cfRule type="cellIs" dxfId="23" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="71" priority="9" operator="equal">
       <formula>10</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E11 G11 I11 K11 M11 O11 Q11 S11">
-    <cfRule type="cellIs" dxfId="22" priority="2" operator="between">
+    <cfRule type="cellIs" dxfId="70" priority="10" operator="between">
       <formula>9.99</formula>
       <formula>9</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E11 G11 I11 K11 M11 O11 Q11 S11">
-    <cfRule type="cellIs" dxfId="21" priority="3" operator="between">
+    <cfRule type="cellIs" dxfId="69" priority="11" operator="between">
       <formula>8.99</formula>
       <formula>8</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E11 G11 I11 K11 M11 O11 Q11 S11">
-    <cfRule type="cellIs" dxfId="20" priority="4" operator="between">
+    <cfRule type="cellIs" dxfId="68" priority="12" operator="between">
       <formula>7.99</formula>
       <formula>7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E11 G11 I11 K11 M11 O11 Q11 S11">
-    <cfRule type="cellIs" dxfId="19" priority="5" operator="between">
+    <cfRule type="cellIs" dxfId="67" priority="13" operator="between">
       <formula>6.99</formula>
       <formula>6</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E11 G11 I11 K11 M11 O11 Q11 S11">
-    <cfRule type="cellIs" dxfId="18" priority="6" operator="between">
+    <cfRule type="cellIs" dxfId="66" priority="14" operator="between">
       <formula>5.99</formula>
       <formula>5.5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E11 G11 I11 K11 M11 O11 Q11 S11">
-    <cfRule type="cellIs" dxfId="17" priority="7" operator="between">
+    <cfRule type="cellIs" dxfId="65" priority="15" operator="between">
       <formula>5.49</formula>
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E11 G11 I11 K11 M11 O11 Q11 S11">
-    <cfRule type="cellIs" dxfId="16" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="64" priority="16" operator="equal">
+      <formula>"NA"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E7 G7 I7 K7 M7 O7 Q7 S7">
+    <cfRule type="cellIs" dxfId="63" priority="1" operator="equal">
+      <formula>10</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E7 G7 I7 K7 M7 O7 Q7 S7">
+    <cfRule type="cellIs" dxfId="62" priority="2" operator="between">
+      <formula>9.99</formula>
+      <formula>9</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E7 G7 I7 K7 M7 O7 Q7 S7">
+    <cfRule type="cellIs" dxfId="61" priority="3" operator="between">
+      <formula>8.99</formula>
+      <formula>8</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E7 G7 I7 K7 M7 O7 Q7 S7">
+    <cfRule type="cellIs" dxfId="60" priority="4" operator="between">
+      <formula>7.99</formula>
+      <formula>7</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E7 G7 I7 K7 M7 O7 Q7 S7">
+    <cfRule type="cellIs" dxfId="59" priority="5" operator="between">
+      <formula>6.99</formula>
+      <formula>6</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E7 G7 I7 K7 M7 O7 Q7 S7">
+    <cfRule type="cellIs" dxfId="58" priority="6" operator="between">
+      <formula>5.99</formula>
+      <formula>5.5</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E7 G7 I7 K7 M7 O7 Q7 S7">
+    <cfRule type="cellIs" dxfId="57" priority="7" operator="between">
+      <formula>5.49</formula>
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E7 G7 I7 K7 M7 O7 Q7 S7">
+    <cfRule type="cellIs" dxfId="56" priority="8" operator="equal">
       <formula>"NA"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2909,36 +3742,42 @@
   <pageSetup pageOrder="overThenDown" orientation="landscape" cellComments="atEnd" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="5">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="6">
         <x14:dataValidation type="list" allowBlank="1" xr:uid="{00000000-0002-0000-0000-000000000000}">
           <x14:formula1>
             <xm:f>Data!$A$2:$A$9</xm:f>
           </x14:formula1>
-          <xm:sqref>I12:I16 K12:K16 M12:M16 O12:O16 Q12:Q16 S12:S16 U12:U16 W12:W16 E12:E16 S8 Q8 O8 M8 K8 I8 G8 E8 W8 U8 G12:G16</xm:sqref>
+          <xm:sqref>I12:I16 K12:K16 M12:M16 O12:O16 Q12:Q16 S12:S16 U12:U16 W12:W16 E12:E16 G12:G16</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" xr:uid="{E63D5A7E-6F1C-47C6-B47D-1FDB9AD75B60}">
+        <x14:dataValidation type="list" allowBlank="1" xr:uid="{1161C697-BE4E-4CF5-8019-BCCD17EB2718}">
           <x14:formula1>
             <xm:f>'I:\Y2\Block 3\Project startup\Design Docs\[PeerReview_ArjendeAldrey.xlsx]Data'!#REF!</xm:f>
           </x14:formula1>
           <xm:sqref>E10 G10 I10 K10 M10 O10 Q10 S10 U10 W10</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" xr:uid="{CA525BAC-F289-433F-A4B1-1094EE328182}">
+        <x14:dataValidation type="list" allowBlank="1" xr:uid="{D7ABF77E-6B4B-48E3-BF45-BA0AF8CC3417}">
           <x14:formula1>
             <xm:f>'I:\Y2\Block 3\Project startup\Design Docs\[PeerReview_Rob.xlsx]Data'!#REF!</xm:f>
           </x14:formula1>
           <xm:sqref>E7 G7 I7 K7 M7 O7 Q7 S7 U7 W7</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" xr:uid="{DB193587-6E1A-4D95-85BF-3FD174764E62}">
+        <x14:dataValidation type="list" allowBlank="1" xr:uid="{493EC00B-FCF5-408D-98AD-55D756DEB96A}">
           <x14:formula1>
             <xm:f>'I:\Y2\Block 3\Project startup\Design Docs\[PeerReview-Humam.xlsx]Data'!#REF!</xm:f>
           </x14:formula1>
           <xm:sqref>E9 G9 I9 K9 M9 O9 Q9 S9 U9 W9</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" xr:uid="{DE79D871-36A9-4F36-A38E-D392AA9D52C0}">
+        <x14:dataValidation type="list" allowBlank="1" xr:uid="{5D027BDF-208D-4867-9F10-04F8F18B5572}">
           <x14:formula1>
-            <xm:f>[PeerReviewGlyn.xlsx]Data!#REF!</xm:f>
+            <xm:f>'I:\Y2\Block 3\Project startup\Team Docs\[PeerReviewGlyn.xlsx]Data'!#REF!</xm:f>
           </x14:formula1>
           <xm:sqref>E11 G11 I11 K11 M11 O11 Q11 S11 U11 W11</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" xr:uid="{52246BAC-375D-4811-841F-2240B4E3A26E}">
+          <x14:formula1>
+            <xm:f>'I:\Y2\Block 3\Project startup\Team Docs\[PeerReview_Tanya.xlsx]Data'!#REF!</xm:f>
+          </x14:formula1>
+          <xm:sqref>S8 Q8 O8 M8 K8 I8 G8 E8 W8 U8</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2947,41 +3786,42 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
-    <pageSetUpPr fitToPage="1"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5FC9082-CAE4-466C-841B-C98B78D1D1C4}">
   <dimension ref="A1:Z18"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="H4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="J7" sqref="J7"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.44140625" customWidth="1"/>
-    <col min="2" max="2" width="8.109375" customWidth="1"/>
-    <col min="3" max="3" width="13.109375" customWidth="1"/>
-    <col min="4" max="4" width="16" customWidth="1"/>
-    <col min="5" max="5" width="5.109375" customWidth="1"/>
-    <col min="6" max="6" width="14.6640625" customWidth="1"/>
-    <col min="7" max="7" width="5.109375" customWidth="1"/>
-    <col min="8" max="8" width="14.6640625" customWidth="1"/>
-    <col min="9" max="9" width="5.109375" customWidth="1"/>
-    <col min="10" max="10" width="14.6640625" customWidth="1"/>
-    <col min="11" max="11" width="5.109375" customWidth="1"/>
-    <col min="12" max="12" width="14.6640625" customWidth="1"/>
-    <col min="13" max="13" width="5.109375" customWidth="1"/>
-    <col min="14" max="14" width="14.6640625" customWidth="1"/>
-    <col min="15" max="15" width="5.109375" customWidth="1"/>
-    <col min="16" max="16" width="14.6640625" customWidth="1"/>
-    <col min="17" max="17" width="5.109375" customWidth="1"/>
-    <col min="18" max="18" width="14.6640625" customWidth="1"/>
-    <col min="19" max="19" width="5.109375" customWidth="1"/>
-    <col min="20" max="20" width="14.6640625" customWidth="1"/>
-    <col min="21" max="21" width="5.109375" customWidth="1"/>
-    <col min="22" max="22" width="15.6640625" customWidth="1"/>
-    <col min="23" max="23" width="5.109375" customWidth="1"/>
-    <col min="24" max="24" width="2.6640625" customWidth="1"/>
+    <col min="1" max="1" width="7.5546875" style="47" customWidth="1"/>
+    <col min="2" max="2" width="8.109375" style="47" customWidth="1"/>
+    <col min="3" max="3" width="18.44140625" style="47" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="50.6640625" style="47" customWidth="1"/>
+    <col min="5" max="5" width="6.6640625" style="47" customWidth="1"/>
+    <col min="6" max="6" width="50.6640625" style="47" customWidth="1"/>
+    <col min="7" max="7" width="6.6640625" style="47" customWidth="1"/>
+    <col min="8" max="8" width="50.6640625" style="47" customWidth="1"/>
+    <col min="9" max="9" width="6.6640625" style="47" customWidth="1"/>
+    <col min="10" max="10" width="50.6640625" style="47" customWidth="1"/>
+    <col min="11" max="11" width="6.6640625" style="47" customWidth="1"/>
+    <col min="12" max="12" width="50.6640625" style="47" customWidth="1"/>
+    <col min="13" max="13" width="6.6640625" style="47" customWidth="1"/>
+    <col min="14" max="14" width="50.6640625" style="47" customWidth="1"/>
+    <col min="15" max="15" width="6.6640625" style="47" customWidth="1"/>
+    <col min="16" max="16" width="14.6640625" style="47" customWidth="1"/>
+    <col min="17" max="17" width="5.109375" style="47" customWidth="1"/>
+    <col min="18" max="18" width="14.6640625" style="47" customWidth="1"/>
+    <col min="19" max="19" width="5.109375" style="47" customWidth="1"/>
+    <col min="20" max="20" width="14.6640625" style="47" customWidth="1"/>
+    <col min="21" max="21" width="5.109375" style="47" customWidth="1"/>
+    <col min="22" max="22" width="15.6640625" style="47" customWidth="1"/>
+    <col min="23" max="23" width="5.109375" style="47" customWidth="1"/>
+    <col min="24" max="24" width="2.6640625" style="47" customWidth="1"/>
+    <col min="25" max="25" width="42" style="47" customWidth="1"/>
+    <col min="26" max="26" width="42.109375" style="47" customWidth="1"/>
+    <col min="27" max="16384" width="14.44140625" style="47"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2992,104 +3832,108 @@
         <v>1</v>
       </c>
       <c r="C1" s="2"/>
-      <c r="D1" s="47" t="s">
+      <c r="D1" s="48" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="48"/>
-      <c r="F1" s="48"/>
-      <c r="G1" s="48"/>
-      <c r="H1" s="48"/>
-      <c r="I1" s="48"/>
-      <c r="J1" s="48"/>
-      <c r="K1" s="48"/>
-      <c r="L1" s="48"/>
-      <c r="M1" s="48"/>
-      <c r="N1" s="48"/>
-      <c r="O1" s="48"/>
-      <c r="P1" s="48"/>
-      <c r="Q1" s="48"/>
-      <c r="R1" s="48"/>
-      <c r="S1" s="48"/>
-      <c r="T1" s="48"/>
-      <c r="U1" s="49"/>
-      <c r="V1" s="56" t="s">
+      <c r="E1" s="49"/>
+      <c r="F1" s="49"/>
+      <c r="G1" s="49"/>
+      <c r="H1" s="49"/>
+      <c r="I1" s="49"/>
+      <c r="J1" s="49"/>
+      <c r="K1" s="49"/>
+      <c r="L1" s="49"/>
+      <c r="M1" s="49"/>
+      <c r="N1" s="49"/>
+      <c r="O1" s="49"/>
+      <c r="P1" s="49"/>
+      <c r="Q1" s="49"/>
+      <c r="R1" s="49"/>
+      <c r="S1" s="49"/>
+      <c r="T1" s="49"/>
+      <c r="U1" s="50"/>
+      <c r="V1" s="57" t="s">
         <v>3</v>
       </c>
-      <c r="W1" s="48"/>
-      <c r="X1" s="48"/>
-      <c r="Y1" s="48"/>
-      <c r="Z1" s="48"/>
+      <c r="W1" s="49"/>
+      <c r="X1" s="49"/>
+      <c r="Y1" s="49"/>
+      <c r="Z1" s="49"/>
     </row>
     <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="4"/>
+      <c r="B2" s="5">
+        <v>12</v>
+      </c>
       <c r="C2" s="5"/>
-      <c r="D2" s="50" t="s">
+      <c r="D2" s="51" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="51"/>
-      <c r="F2" s="51"/>
-      <c r="G2" s="51"/>
-      <c r="H2" s="51"/>
-      <c r="I2" s="51"/>
-      <c r="J2" s="51"/>
-      <c r="K2" s="51"/>
-      <c r="L2" s="51"/>
-      <c r="M2" s="51"/>
-      <c r="N2" s="51"/>
-      <c r="O2" s="51"/>
-      <c r="P2" s="51"/>
-      <c r="Q2" s="51"/>
-      <c r="R2" s="51"/>
-      <c r="S2" s="51"/>
-      <c r="T2" s="51"/>
-      <c r="U2" s="52"/>
-      <c r="V2" s="57"/>
-      <c r="W2" s="51"/>
-      <c r="X2" s="51"/>
-      <c r="Y2" s="51"/>
-      <c r="Z2" s="51"/>
-    </row>
-    <row r="3" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E2" s="52"/>
+      <c r="F2" s="52"/>
+      <c r="G2" s="52"/>
+      <c r="H2" s="52"/>
+      <c r="I2" s="52"/>
+      <c r="J2" s="52"/>
+      <c r="K2" s="52"/>
+      <c r="L2" s="52"/>
+      <c r="M2" s="52"/>
+      <c r="N2" s="52"/>
+      <c r="O2" s="52"/>
+      <c r="P2" s="52"/>
+      <c r="Q2" s="52"/>
+      <c r="R2" s="52"/>
+      <c r="S2" s="52"/>
+      <c r="T2" s="52"/>
+      <c r="U2" s="53"/>
+      <c r="V2" s="58"/>
+      <c r="W2" s="52"/>
+      <c r="X2" s="52"/>
+      <c r="Y2" s="52"/>
+      <c r="Z2" s="52"/>
+    </row>
+    <row r="3" spans="1:26" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="8"/>
-      <c r="D3" s="53" t="s">
+      <c r="C3" s="41" t="s">
+        <v>48</v>
+      </c>
+      <c r="D3" s="54" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="54"/>
-      <c r="F3" s="54"/>
-      <c r="G3" s="54"/>
-      <c r="H3" s="54"/>
-      <c r="I3" s="54"/>
-      <c r="J3" s="54"/>
-      <c r="K3" s="54"/>
-      <c r="L3" s="54"/>
-      <c r="M3" s="54"/>
-      <c r="N3" s="54"/>
-      <c r="O3" s="54"/>
-      <c r="P3" s="54"/>
-      <c r="Q3" s="54"/>
-      <c r="R3" s="54"/>
-      <c r="S3" s="54"/>
-      <c r="T3" s="54"/>
-      <c r="U3" s="55"/>
-      <c r="V3" s="58"/>
-      <c r="W3" s="54"/>
-      <c r="X3" s="54"/>
-      <c r="Y3" s="54"/>
-      <c r="Z3" s="54"/>
+      <c r="E3" s="55"/>
+      <c r="F3" s="55"/>
+      <c r="G3" s="55"/>
+      <c r="H3" s="55"/>
+      <c r="I3" s="55"/>
+      <c r="J3" s="55"/>
+      <c r="K3" s="55"/>
+      <c r="L3" s="55"/>
+      <c r="M3" s="55"/>
+      <c r="N3" s="55"/>
+      <c r="O3" s="55"/>
+      <c r="P3" s="55"/>
+      <c r="Q3" s="55"/>
+      <c r="R3" s="55"/>
+      <c r="S3" s="55"/>
+      <c r="T3" s="55"/>
+      <c r="U3" s="56"/>
+      <c r="V3" s="59"/>
+      <c r="W3" s="55"/>
+      <c r="X3" s="55"/>
+      <c r="Y3" s="55"/>
+      <c r="Z3" s="55"/>
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="9"/>
-      <c r="B4" s="10"/>
-      <c r="C4" s="10"/>
+      <c r="A4" s="11"/>
+      <c r="B4" s="13"/>
+      <c r="C4" s="13"/>
       <c r="D4" s="11" t="s">
         <v>9</v>
       </c>
@@ -3142,46 +3986,46 @@
         <v>18</v>
       </c>
       <c r="U4" s="15"/>
-      <c r="V4" s="10"/>
+      <c r="V4" s="13"/>
       <c r="W4" s="15"/>
-      <c r="X4" s="10"/>
-      <c r="Y4" s="10"/>
-      <c r="Z4" s="10"/>
-    </row>
-    <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="9"/>
-      <c r="B5" s="10"/>
-      <c r="C5" s="10"/>
-      <c r="D5" s="63" t="s">
+      <c r="X4" s="13"/>
+      <c r="Y4" s="13"/>
+      <c r="Z4" s="13"/>
+    </row>
+    <row r="5" spans="1:26" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="11"/>
+      <c r="B5" s="13"/>
+      <c r="C5" s="13"/>
+      <c r="D5" s="64" t="s">
         <v>19</v>
       </c>
-      <c r="E5" s="51"/>
-      <c r="F5" s="51"/>
-      <c r="G5" s="51"/>
-      <c r="H5" s="51"/>
-      <c r="I5" s="51"/>
-      <c r="J5" s="51"/>
-      <c r="K5" s="51"/>
-      <c r="L5" s="51"/>
-      <c r="M5" s="51"/>
-      <c r="N5" s="51"/>
-      <c r="O5" s="51"/>
-      <c r="P5" s="51"/>
-      <c r="Q5" s="51"/>
-      <c r="R5" s="51"/>
-      <c r="S5" s="51"/>
-      <c r="T5" s="51"/>
-      <c r="U5" s="51"/>
-      <c r="V5" s="51"/>
-      <c r="W5" s="51"/>
-      <c r="X5" s="10"/>
+      <c r="E5" s="52"/>
+      <c r="F5" s="52"/>
+      <c r="G5" s="52"/>
+      <c r="H5" s="52"/>
+      <c r="I5" s="52"/>
+      <c r="J5" s="52"/>
+      <c r="K5" s="52"/>
+      <c r="L5" s="52"/>
+      <c r="M5" s="52"/>
+      <c r="N5" s="52"/>
+      <c r="O5" s="52"/>
+      <c r="P5" s="52"/>
+      <c r="Q5" s="52"/>
+      <c r="R5" s="52"/>
+      <c r="S5" s="52"/>
+      <c r="T5" s="52"/>
+      <c r="U5" s="52"/>
+      <c r="V5" s="52"/>
+      <c r="W5" s="52"/>
+      <c r="X5" s="13"/>
       <c r="Y5" s="16" t="s">
         <v>20</v>
       </c>
       <c r="Z5" s="16"/>
     </row>
     <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="9"/>
+      <c r="A6" s="11"/>
       <c r="B6" s="17" t="s">
         <v>21</v>
       </c>
@@ -3190,42 +4034,42 @@
       </c>
       <c r="D6" s="18" t="str">
         <f>CONCATENATE("Review of ",C7)</f>
-        <v>Review of Team Member 1</v>
+        <v>Review of Rob O'Connor</v>
       </c>
       <c r="E6" s="19" t="s">
         <v>23</v>
       </c>
       <c r="F6" s="18" t="str">
         <f>CONCATENATE("Review of ",C8)</f>
-        <v>Review of Team Member 2</v>
+        <v>Review of Tanya Schrijver</v>
       </c>
       <c r="G6" s="19" t="s">
         <v>23</v>
       </c>
       <c r="H6" s="18" t="str">
         <f>CONCATENATE("Review of ",C9)</f>
-        <v>Review of Team Member 3</v>
+        <v>Review of Humam Abud Allah</v>
       </c>
       <c r="I6" s="19" t="s">
         <v>23</v>
       </c>
       <c r="J6" s="18" t="str">
         <f>CONCATENATE("Review of ",C10)</f>
-        <v>Review of Team Member 4</v>
+        <v>Review of Arjen de Aldrey</v>
       </c>
       <c r="K6" s="19" t="s">
         <v>23</v>
       </c>
       <c r="L6" s="18" t="str">
         <f>CONCATENATE("Review of ",C11)</f>
-        <v>Review of Team Member 5</v>
+        <v>Review of Glyn Leine</v>
       </c>
       <c r="M6" s="19" t="s">
         <v>23</v>
       </c>
       <c r="N6" s="18" t="str">
         <f>CONCATENATE("Review of ",C12)</f>
-        <v>Review of Team Member 6</v>
+        <v>Review of Rowan Ramsey</v>
       </c>
       <c r="O6" s="19" t="s">
         <v>23</v>
@@ -3258,7 +4102,7 @@
       <c r="W6" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="X6" s="10"/>
+      <c r="X6" s="13"/>
       <c r="Y6" s="16" t="s">
         <v>24</v>
       </c>
@@ -3266,40 +4110,52 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="62" t="s">
+    <row r="7" spans="1:26" s="46" customFormat="1" ht="100.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="63" t="s">
         <v>26</v>
       </c>
       <c r="B7" s="20">
-        <v>12335</v>
+        <v>445921</v>
       </c>
       <c r="C7" s="21" t="s">
-        <v>27</v>
+        <v>49</v>
       </c>
       <c r="D7" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="E7" s="23"/>
+        <v>109</v>
+      </c>
+      <c r="E7" s="42">
+        <v>7</v>
+      </c>
       <c r="F7" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="G7" s="24"/>
+        <v>110</v>
+      </c>
+      <c r="G7" s="42">
+        <v>8</v>
+      </c>
       <c r="H7" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="I7" s="24"/>
+        <v>111</v>
+      </c>
+      <c r="I7" s="42">
+        <v>8</v>
+      </c>
       <c r="J7" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="K7" s="24"/>
+        <v>114</v>
+      </c>
+      <c r="K7" s="42">
+        <v>8</v>
+      </c>
       <c r="L7" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="M7" s="24"/>
+        <v>113</v>
+      </c>
+      <c r="M7" s="24">
+        <v>8</v>
+      </c>
       <c r="N7" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="O7" s="24"/>
+        <v>112</v>
+      </c>
+      <c r="O7" s="24">
+        <v>7</v>
+      </c>
       <c r="P7" s="22" t="s">
         <v>28</v>
       </c>
@@ -3317,93 +4173,117 @@
       </c>
       <c r="W7" s="24"/>
       <c r="X7" s="25"/>
-      <c r="Y7" s="26"/>
-      <c r="Z7" s="27"/>
-    </row>
-    <row r="8" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="51"/>
+      <c r="Y7" s="44"/>
+      <c r="Z7" s="45"/>
+    </row>
+    <row r="8" spans="1:26" s="46" customFormat="1" ht="100.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="52"/>
       <c r="B8" s="20">
-        <v>12335</v>
+        <v>464704</v>
       </c>
       <c r="C8" s="21" t="s">
-        <v>29</v>
-      </c>
-      <c r="D8" s="28" t="s">
-        <v>28</v>
-      </c>
-      <c r="E8" s="29"/>
-      <c r="F8" s="28" t="s">
-        <v>28</v>
-      </c>
-      <c r="G8" s="29"/>
-      <c r="H8" s="28" t="s">
-        <v>28</v>
-      </c>
-      <c r="I8" s="29"/>
-      <c r="J8" s="28" t="s">
-        <v>28</v>
-      </c>
-      <c r="K8" s="29"/>
+        <v>50</v>
+      </c>
+      <c r="D8" s="22" t="s">
+        <v>95</v>
+      </c>
+      <c r="E8" s="43">
+        <v>8</v>
+      </c>
+      <c r="F8" s="22" t="s">
+        <v>96</v>
+      </c>
+      <c r="G8" s="43">
+        <v>7</v>
+      </c>
+      <c r="H8" s="22" t="s">
+        <v>97</v>
+      </c>
+      <c r="I8" s="43">
+        <v>7</v>
+      </c>
+      <c r="J8" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="K8" s="43">
+        <v>7</v>
+      </c>
       <c r="L8" s="28" t="s">
-        <v>28</v>
-      </c>
-      <c r="M8" s="29"/>
+        <v>98</v>
+      </c>
+      <c r="M8" s="30">
+        <v>7</v>
+      </c>
       <c r="N8" s="28" t="s">
-        <v>28</v>
-      </c>
-      <c r="O8" s="29"/>
+        <v>98</v>
+      </c>
+      <c r="O8" s="30">
+        <v>7</v>
+      </c>
       <c r="P8" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="Q8" s="29"/>
+      <c r="Q8" s="30"/>
       <c r="R8" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="S8" s="29"/>
+      <c r="S8" s="30"/>
       <c r="T8" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="U8" s="29"/>
+      <c r="U8" s="30"/>
       <c r="V8" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="W8" s="29"/>
+      <c r="W8" s="30"/>
       <c r="X8" s="25"/>
       <c r="Y8" s="26"/>
       <c r="Z8" s="27"/>
     </row>
-    <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="51"/>
+    <row r="9" spans="1:26" s="46" customFormat="1" ht="100.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="52"/>
       <c r="B9" s="20">
-        <v>12335</v>
+        <v>428729</v>
       </c>
       <c r="C9" s="21" t="s">
-        <v>30</v>
-      </c>
-      <c r="D9" s="22" t="s">
-        <v>31</v>
-      </c>
-      <c r="E9" s="24"/>
-      <c r="F9" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="G9" s="24"/>
-      <c r="H9" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="I9" s="24"/>
-      <c r="J9" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="K9" s="24"/>
-      <c r="L9" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="M9" s="24"/>
-      <c r="N9" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="O9" s="24"/>
+        <v>51</v>
+      </c>
+      <c r="D9" s="40" t="s">
+        <v>103</v>
+      </c>
+      <c r="E9" s="42">
+        <v>10</v>
+      </c>
+      <c r="F9" s="40" t="s">
+        <v>104</v>
+      </c>
+      <c r="G9" s="42">
+        <v>10</v>
+      </c>
+      <c r="H9" s="40" t="s">
+        <v>105</v>
+      </c>
+      <c r="I9" s="42">
+        <v>7</v>
+      </c>
+      <c r="J9" s="40" t="s">
+        <v>106</v>
+      </c>
+      <c r="K9" s="42">
+        <v>10</v>
+      </c>
+      <c r="L9" s="40" t="s">
+        <v>107</v>
+      </c>
+      <c r="M9" s="24">
+        <v>10</v>
+      </c>
+      <c r="N9" s="40" t="s">
+        <v>108</v>
+      </c>
+      <c r="O9" s="24">
+        <v>10</v>
+      </c>
       <c r="P9" s="22" t="s">
         <v>28</v>
       </c>
@@ -3421,93 +4301,119 @@
       </c>
       <c r="W9" s="24"/>
       <c r="X9" s="25"/>
-      <c r="Y9" s="26"/>
+      <c r="Y9" s="26" t="s">
+        <v>94</v>
+      </c>
       <c r="Z9" s="27"/>
     </row>
-    <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="51"/>
+    <row r="10" spans="1:26" s="46" customFormat="1" ht="100.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="52"/>
       <c r="B10" s="20">
-        <v>12335</v>
+        <v>444711</v>
       </c>
       <c r="C10" s="21" t="s">
-        <v>32</v>
-      </c>
-      <c r="D10" s="28" t="s">
-        <v>28</v>
-      </c>
-      <c r="E10" s="30"/>
-      <c r="F10" s="28" t="s">
-        <v>28</v>
-      </c>
-      <c r="G10" s="29"/>
-      <c r="H10" s="28" t="s">
-        <v>28</v>
-      </c>
-      <c r="I10" s="29"/>
-      <c r="J10" s="28" t="s">
-        <v>28</v>
-      </c>
-      <c r="K10" s="29"/>
+        <v>52</v>
+      </c>
+      <c r="D10" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="E10" s="43">
+        <v>8</v>
+      </c>
+      <c r="F10" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="G10" s="43">
+        <v>7</v>
+      </c>
+      <c r="H10" s="22" t="s">
+        <v>99</v>
+      </c>
+      <c r="I10" s="43">
+        <v>7</v>
+      </c>
+      <c r="J10" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="K10" s="43">
+        <v>7</v>
+      </c>
       <c r="L10" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="M10" s="29"/>
+      <c r="M10" s="30">
+        <v>8</v>
+      </c>
       <c r="N10" s="28" t="s">
-        <v>28</v>
-      </c>
-      <c r="O10" s="29"/>
+        <v>100</v>
+      </c>
+      <c r="O10" s="30">
+        <v>7</v>
+      </c>
       <c r="P10" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="Q10" s="29"/>
+      <c r="Q10" s="30"/>
       <c r="R10" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="S10" s="29"/>
+      <c r="S10" s="30"/>
       <c r="T10" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="U10" s="29"/>
+      <c r="U10" s="30"/>
       <c r="V10" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="W10" s="29"/>
+      <c r="W10" s="30"/>
       <c r="X10" s="25"/>
       <c r="Y10" s="26"/>
       <c r="Z10" s="27"/>
     </row>
-    <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="51"/>
+    <row r="11" spans="1:26" s="46" customFormat="1" ht="100.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="52"/>
       <c r="B11" s="20">
-        <v>12335</v>
+        <v>445021</v>
       </c>
       <c r="C11" s="21" t="s">
-        <v>33</v>
+        <v>47</v>
       </c>
       <c r="D11" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="E11" s="24"/>
+        <v>98</v>
+      </c>
+      <c r="E11" s="24">
+        <v>8</v>
+      </c>
       <c r="F11" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="G11" s="24"/>
-      <c r="H11" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="I11" s="24"/>
+        <v>101</v>
+      </c>
+      <c r="G11" s="24">
+        <v>8</v>
+      </c>
+      <c r="H11" s="40" t="s">
+        <v>98</v>
+      </c>
+      <c r="I11" s="24">
+        <v>8</v>
+      </c>
       <c r="J11" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="K11" s="24"/>
+        <v>98</v>
+      </c>
+      <c r="K11" s="24">
+        <v>8</v>
+      </c>
       <c r="L11" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="M11" s="24"/>
+        <v>98</v>
+      </c>
+      <c r="M11" s="24">
+        <v>7</v>
+      </c>
       <c r="N11" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="O11" s="24"/>
+        <v>102</v>
+      </c>
+      <c r="O11" s="24">
+        <v>8</v>
+      </c>
       <c r="P11" s="22" t="s">
         <v>28</v>
       </c>
@@ -3528,13 +4434,13 @@
       <c r="Y11" s="26"/>
       <c r="Z11" s="27"/>
     </row>
-    <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="51"/>
+    <row r="12" spans="1:26" ht="100.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="52"/>
       <c r="B12" s="20">
-        <v>12335</v>
+        <v>459575</v>
       </c>
       <c r="C12" s="21" t="s">
-        <v>34</v>
+        <v>53</v>
       </c>
       <c r="D12" s="28" t="s">
         <v>28</v>
@@ -3543,45 +4449,45 @@
       <c r="F12" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="G12" s="29"/>
+      <c r="G12" s="30"/>
       <c r="H12" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="I12" s="29"/>
+      <c r="I12" s="30"/>
       <c r="J12" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="K12" s="29"/>
+      <c r="K12" s="30"/>
       <c r="L12" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="M12" s="29"/>
+      <c r="M12" s="30"/>
       <c r="N12" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="O12" s="29"/>
+      <c r="O12" s="30"/>
       <c r="P12" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="Q12" s="29"/>
+      <c r="Q12" s="30"/>
       <c r="R12" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="S12" s="29"/>
+      <c r="S12" s="30"/>
       <c r="T12" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="U12" s="29"/>
+      <c r="U12" s="30"/>
       <c r="V12" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="W12" s="29"/>
+      <c r="W12" s="30"/>
       <c r="X12" s="25"/>
       <c r="Y12" s="26"/>
       <c r="Z12" s="27"/>
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="51"/>
+      <c r="A13" s="52"/>
       <c r="B13" s="20">
         <v>12335</v>
       </c>
@@ -3633,7 +4539,7 @@
       <c r="Z13" s="27"/>
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="51"/>
+      <c r="A14" s="52"/>
       <c r="B14" s="20">
         <v>12335</v>
       </c>
@@ -3643,49 +4549,49 @@
       <c r="D14" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="E14" s="29"/>
+      <c r="E14" s="30"/>
       <c r="F14" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="G14" s="29"/>
+      <c r="G14" s="30"/>
       <c r="H14" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="I14" s="29"/>
+      <c r="I14" s="30"/>
       <c r="J14" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="K14" s="29"/>
+      <c r="K14" s="30"/>
       <c r="L14" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="M14" s="29"/>
+      <c r="M14" s="30"/>
       <c r="N14" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="O14" s="29"/>
+      <c r="O14" s="30"/>
       <c r="P14" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="Q14" s="29"/>
+      <c r="Q14" s="30"/>
       <c r="R14" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="S14" s="29"/>
+      <c r="S14" s="30"/>
       <c r="T14" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="U14" s="29"/>
+      <c r="U14" s="30"/>
       <c r="V14" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="W14" s="29"/>
+      <c r="W14" s="30"/>
       <c r="X14" s="25"/>
       <c r="Y14" s="26"/>
       <c r="Z14" s="27"/>
     </row>
     <row r="15" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="51"/>
+      <c r="A15" s="52"/>
       <c r="B15" s="20">
         <v>12335</v>
       </c>
@@ -3737,7 +4643,7 @@
       <c r="Z15" s="27"/>
     </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="51"/>
+      <c r="A16" s="52"/>
       <c r="B16" s="20">
         <v>12335</v>
       </c>
@@ -3751,39 +4657,39 @@
       <c r="F16" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="G16" s="29"/>
+      <c r="G16" s="30"/>
       <c r="H16" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="I16" s="29"/>
+      <c r="I16" s="30"/>
       <c r="J16" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="K16" s="29"/>
+      <c r="K16" s="30"/>
       <c r="L16" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="M16" s="29"/>
+      <c r="M16" s="30"/>
       <c r="N16" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="O16" s="29"/>
+      <c r="O16" s="30"/>
       <c r="P16" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="Q16" s="29"/>
+      <c r="Q16" s="30"/>
       <c r="R16" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="S16" s="29"/>
+      <c r="S16" s="30"/>
       <c r="T16" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="U16" s="29"/>
+      <c r="U16" s="30"/>
       <c r="V16" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="W16" s="29"/>
+      <c r="W16" s="30"/>
       <c r="X16" s="25"/>
       <c r="Y16" s="26"/>
       <c r="Z16" s="27"/>
@@ -3795,44 +4701,44 @@
       <c r="D17" s="31" t="s">
         <v>39</v>
       </c>
-      <c r="E17" s="33" t="str">
+      <c r="E17" s="33">
         <f>IF(COUNTA(E7:E16)&gt;0,COUNT(E7:E16)/COUNTA(E7:E16),"NA")</f>
-        <v>NA</v>
+        <v>1</v>
       </c>
       <c r="F17" s="31" t="s">
         <v>39</v>
       </c>
-      <c r="G17" s="33" t="str">
+      <c r="G17" s="33">
         <f>IF(COUNTA(G7:G16)&gt;0,COUNT(G7:G16)/COUNTA(G7:G16),"NA")</f>
-        <v>NA</v>
+        <v>1</v>
       </c>
       <c r="H17" s="31" t="s">
         <v>39</v>
       </c>
-      <c r="I17" s="33" t="str">
+      <c r="I17" s="33">
         <f>IF(COUNTA(I7:I16)&gt;0,COUNT(I7:I16)/COUNTA(I7:I16),"NA")</f>
-        <v>NA</v>
+        <v>1</v>
       </c>
       <c r="J17" s="31" t="s">
         <v>39</v>
       </c>
-      <c r="K17" s="33" t="str">
+      <c r="K17" s="33">
         <f>IF(COUNTA(K7:K16)&gt;0,COUNT(K7:K16)/COUNTA(K7:K16),"NA")</f>
-        <v>NA</v>
+        <v>1</v>
       </c>
       <c r="L17" s="31" t="s">
         <v>39</v>
       </c>
-      <c r="M17" s="33" t="str">
+      <c r="M17" s="33">
         <f>IF(COUNTA(M7:M16)&gt;0,COUNT(M7:M16)/COUNTA(M7:M16),"NA")</f>
-        <v>NA</v>
+        <v>1</v>
       </c>
       <c r="N17" s="31" t="s">
         <v>39</v>
       </c>
-      <c r="O17" s="33" t="str">
+      <c r="O17" s="33">
         <f>IF(COUNTA(O7:O16)&gt;0,COUNT(O7:O16)/COUNTA(O7:O16),"NA")</f>
-        <v>NA</v>
+        <v>1</v>
       </c>
       <c r="P17" s="31" t="s">
         <v>39</v>
@@ -3867,102 +4773,361 @@
       <c r="Z17" s="32"/>
     </row>
     <row r="18" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="59" t="s">
+      <c r="A18" s="60" t="s">
         <v>40</v>
       </c>
-      <c r="B18" s="60"/>
-      <c r="C18" s="60"/>
-      <c r="D18" s="60"/>
-      <c r="E18" s="60"/>
-      <c r="F18" s="60"/>
-      <c r="G18" s="60"/>
-      <c r="H18" s="60"/>
-      <c r="I18" s="60"/>
-      <c r="J18" s="60"/>
-      <c r="K18" s="60"/>
-      <c r="L18" s="60"/>
-      <c r="M18" s="60"/>
-      <c r="N18" s="60"/>
-      <c r="O18" s="60"/>
-      <c r="P18" s="60"/>
-      <c r="Q18" s="60"/>
-      <c r="R18" s="60"/>
-      <c r="S18" s="60"/>
-      <c r="T18" s="60"/>
-      <c r="U18" s="60"/>
-      <c r="V18" s="60"/>
-      <c r="W18" s="60"/>
-      <c r="X18" s="60"/>
-      <c r="Y18" s="60"/>
-      <c r="Z18" s="61"/>
+      <c r="B18" s="61"/>
+      <c r="C18" s="61"/>
+      <c r="D18" s="61"/>
+      <c r="E18" s="61"/>
+      <c r="F18" s="61"/>
+      <c r="G18" s="61"/>
+      <c r="H18" s="61"/>
+      <c r="I18" s="61"/>
+      <c r="J18" s="61"/>
+      <c r="K18" s="61"/>
+      <c r="L18" s="61"/>
+      <c r="M18" s="61"/>
+      <c r="N18" s="61"/>
+      <c r="O18" s="61"/>
+      <c r="P18" s="61"/>
+      <c r="Q18" s="61"/>
+      <c r="R18" s="61"/>
+      <c r="S18" s="61"/>
+      <c r="T18" s="61"/>
+      <c r="U18" s="61"/>
+      <c r="V18" s="61"/>
+      <c r="W18" s="61"/>
+      <c r="X18" s="61"/>
+      <c r="Y18" s="61"/>
+      <c r="Z18" s="62"/>
     </row>
   </sheetData>
   <mergeCells count="7">
+    <mergeCell ref="A18:Z18"/>
     <mergeCell ref="D1:U1"/>
+    <mergeCell ref="V1:Z3"/>
     <mergeCell ref="D2:U2"/>
     <mergeCell ref="D3:U3"/>
-    <mergeCell ref="V1:Z3"/>
-    <mergeCell ref="A18:Z18"/>
+    <mergeCell ref="D5:W5"/>
     <mergeCell ref="A7:A16"/>
-    <mergeCell ref="D5:W5"/>
   </mergeCells>
-  <conditionalFormatting sqref="E4 G4 I4 K4 M4 O4 Q4 S4 E7:E17 G7:G17 I7:I17 K7:K17 M7:M17 O7:O17 Q7:Q17 S7:S17 U17 W17">
+  <conditionalFormatting sqref="E4 G4 I4 K4 M4 O4 Q4 S4 U17 W17 S12:S17 Q12:Q17 O12:O17 M12:M17 K12:K17 I12:I17 G12:G17 E12:E17">
+    <cfRule type="cellIs" dxfId="55" priority="41" operator="equal">
+      <formula>10</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E4 G4 I4 K4 M4 O4 Q4 S4 U17 W17 S12:S17 Q12:Q17 O12:O17 M12:M17 K12:K17 I12:I17 G12:G17 E12:E17">
+    <cfRule type="cellIs" dxfId="54" priority="42" operator="between">
+      <formula>9.99</formula>
+      <formula>9</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E4 G4 I4 K4 M4 O4 Q4 S4 U17 W17 S12:S17 Q12:Q17 O12:O17 M12:M17 K12:K17 I12:I17 G12:G17 E12:E17">
+    <cfRule type="cellIs" dxfId="53" priority="43" operator="between">
+      <formula>8.99</formula>
+      <formula>8</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E4 G4 I4 K4 M4 O4 Q4 S4 U17 W17 S12:S17 Q12:Q17 O12:O17 M12:M17 K12:K17 I12:I17 G12:G17 E12:E17">
+    <cfRule type="cellIs" dxfId="52" priority="44" operator="between">
+      <formula>7.99</formula>
+      <formula>7</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E4 G4 I4 K4 M4 O4 Q4 S4 U17 W17 S12:S17 Q12:Q17 O12:O17 M12:M17 K12:K17 I12:I17 G12:G17 E12:E17">
+    <cfRule type="cellIs" dxfId="51" priority="45" operator="between">
+      <formula>6.99</formula>
+      <formula>6</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E4 G4 I4 K4 M4 O4 Q4 S4 U17 W17 S12:S17 Q12:Q17 O12:O17 M12:M17 K12:K17 I12:I17 G12:G17 E12:E17">
+    <cfRule type="cellIs" dxfId="50" priority="46" operator="between">
+      <formula>5.99</formula>
+      <formula>5.5</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E4 G4 I4 K4 M4 O4 Q4 S4 U17 W17 S12:S17 Q12:Q17 O12:O17 M12:M17 K12:K17 I12:I17 G12:G17 E12:E17">
+    <cfRule type="cellIs" dxfId="49" priority="47" operator="between">
+      <formula>5.49</formula>
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E4 G4 I4 K4 M4 O4 Q4 S4 U17 W17 S12:S17 Q12:Q17 O12:O17 M12:M17 K12:K17 I12:I17 G12:G17 E12:E17">
+    <cfRule type="cellIs" dxfId="48" priority="48" operator="equal">
+      <formula>"NA"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E9 G9 I9 K9 M9 O9 Q9 S9">
+    <cfRule type="cellIs" dxfId="47" priority="33" operator="equal">
+      <formula>10</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E9 G9 I9 K9 M9 O9 Q9 S9">
+    <cfRule type="cellIs" dxfId="46" priority="34" operator="between">
+      <formula>9.99</formula>
+      <formula>9</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E9 G9 I9 K9 M9 O9 Q9 S9">
+    <cfRule type="cellIs" dxfId="45" priority="35" operator="between">
+      <formula>8.99</formula>
+      <formula>8</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E9 G9 I9 K9 M9 O9 Q9 S9">
+    <cfRule type="cellIs" dxfId="44" priority="36" operator="between">
+      <formula>7.99</formula>
+      <formula>7</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E9 G9 I9 K9 M9 O9 Q9 S9">
+    <cfRule type="cellIs" dxfId="43" priority="37" operator="between">
+      <formula>6.99</formula>
+      <formula>6</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E9 G9 I9 K9 M9 O9 Q9 S9">
+    <cfRule type="cellIs" dxfId="42" priority="38" operator="between">
+      <formula>5.99</formula>
+      <formula>5.5</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E9 G9 I9 K9 M9 O9 Q9 S9">
+    <cfRule type="cellIs" dxfId="41" priority="39" operator="between">
+      <formula>5.49</formula>
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E9 G9 I9 K9 M9 O9 Q9 S9">
+    <cfRule type="cellIs" dxfId="40" priority="40" operator="equal">
+      <formula>"NA"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E8 G8 I8 K8 M8 O8 Q8 S8">
+    <cfRule type="cellIs" dxfId="39" priority="25" operator="equal">
+      <formula>10</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E8 G8 I8 K8 M8 O8 Q8 S8">
+    <cfRule type="cellIs" dxfId="38" priority="26" operator="between">
+      <formula>9.99</formula>
+      <formula>9</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E8 G8 I8 K8 M8 O8 Q8 S8">
+    <cfRule type="cellIs" dxfId="37" priority="27" operator="between">
+      <formula>8.99</formula>
+      <formula>8</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E8 G8 I8 K8 M8 O8 Q8 S8">
+    <cfRule type="cellIs" dxfId="36" priority="28" operator="between">
+      <formula>7.99</formula>
+      <formula>7</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E8 G8 I8 K8 M8 O8 Q8 S8">
+    <cfRule type="cellIs" dxfId="35" priority="29" operator="between">
+      <formula>6.99</formula>
+      <formula>6</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E8 G8 I8 K8 M8 O8 Q8 S8">
+    <cfRule type="cellIs" dxfId="34" priority="30" operator="between">
+      <formula>5.99</formula>
+      <formula>5.5</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E8 G8 I8 K8 M8 O8 Q8 S8">
+    <cfRule type="cellIs" dxfId="33" priority="31" operator="between">
+      <formula>5.49</formula>
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E8 G8 I8 K8 M8 O8 Q8 S8">
+    <cfRule type="cellIs" dxfId="32" priority="32" operator="equal">
+      <formula>"NA"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E10 G10 I10 K10 M10 O10 Q10 S10">
+    <cfRule type="cellIs" dxfId="31" priority="17" operator="equal">
+      <formula>10</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E10 G10 I10 K10 M10 O10 Q10 S10">
+    <cfRule type="cellIs" dxfId="30" priority="18" operator="between">
+      <formula>9.99</formula>
+      <formula>9</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E10 G10 I10 K10 M10 O10 Q10 S10">
+    <cfRule type="cellIs" dxfId="29" priority="19" operator="between">
+      <formula>8.99</formula>
+      <formula>8</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E10 G10 I10 K10 M10 O10 Q10 S10">
+    <cfRule type="cellIs" dxfId="28" priority="20" operator="between">
+      <formula>7.99</formula>
+      <formula>7</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E10 G10 I10 K10 M10 O10 Q10 S10">
+    <cfRule type="cellIs" dxfId="27" priority="21" operator="between">
+      <formula>6.99</formula>
+      <formula>6</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E10 G10 I10 K10 M10 O10 Q10 S10">
+    <cfRule type="cellIs" dxfId="26" priority="22" operator="between">
+      <formula>5.99</formula>
+      <formula>5.5</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E10 G10 I10 K10 M10 O10 Q10 S10">
+    <cfRule type="cellIs" dxfId="25" priority="23" operator="between">
+      <formula>5.49</formula>
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E10 G10 I10 K10 M10 O10 Q10 S10">
+    <cfRule type="cellIs" dxfId="24" priority="24" operator="equal">
+      <formula>"NA"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E11 G11 I11 K11 M11 O11 Q11 S11">
+    <cfRule type="cellIs" dxfId="23" priority="9" operator="equal">
+      <formula>10</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E11 G11 I11 K11 M11 O11 Q11 S11">
+    <cfRule type="cellIs" dxfId="22" priority="10" operator="between">
+      <formula>9.99</formula>
+      <formula>9</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E11 G11 I11 K11 M11 O11 Q11 S11">
+    <cfRule type="cellIs" dxfId="21" priority="11" operator="between">
+      <formula>8.99</formula>
+      <formula>8</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E11 G11 I11 K11 M11 O11 Q11 S11">
+    <cfRule type="cellIs" dxfId="20" priority="12" operator="between">
+      <formula>7.99</formula>
+      <formula>7</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E11 G11 I11 K11 M11 O11 Q11 S11">
+    <cfRule type="cellIs" dxfId="19" priority="13" operator="between">
+      <formula>6.99</formula>
+      <formula>6</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E11 G11 I11 K11 M11 O11 Q11 S11">
+    <cfRule type="cellIs" dxfId="18" priority="14" operator="between">
+      <formula>5.99</formula>
+      <formula>5.5</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E11 G11 I11 K11 M11 O11 Q11 S11">
+    <cfRule type="cellIs" dxfId="17" priority="15" operator="between">
+      <formula>5.49</formula>
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E11 G11 I11 K11 M11 O11 Q11 S11">
+    <cfRule type="cellIs" dxfId="16" priority="16" operator="equal">
+      <formula>"NA"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E7 G7 I7 K7 M7 O7 Q7 S7">
     <cfRule type="cellIs" dxfId="15" priority="1" operator="equal">
       <formula>10</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E4 G4 I4 K4 M4 O4 Q4 S4 E7:E17 G7:G17 I7:I17 K7:K17 M7:M17 O7:O17 Q7:Q17 S7:S17 U17 W17">
+  <conditionalFormatting sqref="E7 G7 I7 K7 M7 O7 Q7 S7">
     <cfRule type="cellIs" dxfId="14" priority="2" operator="between">
       <formula>9.99</formula>
       <formula>9</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E4 G4 I4 K4 M4 O4 Q4 S4 E7:E17 G7:G17 I7:I17 K7:K17 M7:M17 O7:O17 Q7:Q17 S7:S17 U17 W17">
+  <conditionalFormatting sqref="E7 G7 I7 K7 M7 O7 Q7 S7">
     <cfRule type="cellIs" dxfId="13" priority="3" operator="between">
       <formula>8.99</formula>
       <formula>8</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E4 G4 I4 K4 M4 O4 Q4 S4 E7:E17 G7:G17 I7:I17 K7:K17 M7:M17 O7:O17 Q7:Q17 S7:S17 U17 W17">
+  <conditionalFormatting sqref="E7 G7 I7 K7 M7 O7 Q7 S7">
     <cfRule type="cellIs" dxfId="12" priority="4" operator="between">
       <formula>7.99</formula>
       <formula>7</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E4 G4 I4 K4 M4 O4 Q4 S4 E7:E17 G7:G17 I7:I17 K7:K17 M7:M17 O7:O17 Q7:Q17 S7:S17 U17 W17">
+  <conditionalFormatting sqref="E7 G7 I7 K7 M7 O7 Q7 S7">
     <cfRule type="cellIs" dxfId="11" priority="5" operator="between">
       <formula>6.99</formula>
       <formula>6</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E4 G4 I4 K4 M4 O4 Q4 S4 E7:E17 G7:G17 I7:I17 K7:K17 M7:M17 O7:O17 Q7:Q17 S7:S17 U17 W17">
+  <conditionalFormatting sqref="E7 G7 I7 K7 M7 O7 Q7 S7">
     <cfRule type="cellIs" dxfId="10" priority="6" operator="between">
       <formula>5.99</formula>
       <formula>5.5</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E4 G4 I4 K4 M4 O4 Q4 S4 E7:E17 G7:G17 I7:I17 K7:K17 M7:M17 O7:O17 Q7:Q17 S7:S17 U17 W17">
+  <conditionalFormatting sqref="E7 G7 I7 K7 M7 O7 Q7 S7">
     <cfRule type="cellIs" dxfId="9" priority="7" operator="between">
       <formula>5.49</formula>
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E4 G4 I4 K4 M4 O4 Q4 S4 E7:E17 G7:G17 I7:I17 K7:K17 M7:M17 O7:O17 Q7:Q17 S7:S17 U17 W17">
+  <conditionalFormatting sqref="E7 G7 I7 K7 M7 O7 Q7 S7">
     <cfRule type="cellIs" dxfId="8" priority="8" operator="equal">
       <formula>"NA"</formula>
     </cfRule>
   </conditionalFormatting>
-  <printOptions horizontalCentered="1" gridLines="1"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup pageOrder="overThenDown" orientation="landscape" cellComments="atEnd"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" xr:uid="{00000000-0002-0000-0100-000000000000}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="6">
+        <x14:dataValidation type="list" allowBlank="1" xr:uid="{C898EC94-E6FB-4F99-82BA-726D7C2459BB}">
+          <x14:formula1>
+            <xm:f>'I:\Y2\Block 3\Project startup\Team Docs\[PeerReview_Tanya.xlsx]Data'!#REF!</xm:f>
+          </x14:formula1>
+          <xm:sqref>S8 Q8 O8 M8 K8 I8 G8 E8 W8 U8</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" xr:uid="{6204A054-9525-4CC1-81CD-2AEA85B9C79F}">
+          <x14:formula1>
+            <xm:f>'I:\Y2\Block 3\Project startup\Team Docs\[PeerReviewGlyn.xlsx]Data'!#REF!</xm:f>
+          </x14:formula1>
+          <xm:sqref>E11 G11 I11 K11 M11 O11 Q11 S11 U11 W11</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" xr:uid="{705239EC-713F-4DB0-BFB5-36134D7F6891}">
+          <x14:formula1>
+            <xm:f>'I:\Y2\Block 3\Project startup\Design Docs\[PeerReview-Humam.xlsx]Data'!#REF!</xm:f>
+          </x14:formula1>
+          <xm:sqref>E9 G9 I9 K9 M9 O9 Q9 S9 U9 W9</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" xr:uid="{CC3677BE-2011-4CF6-B613-5164BBC8942E}">
+          <x14:formula1>
+            <xm:f>'I:\Y2\Block 3\Project startup\Design Docs\[PeerReview_Rob.xlsx]Data'!#REF!</xm:f>
+          </x14:formula1>
+          <xm:sqref>E7 G7 I7 K7 M7 O7 Q7 S7 U7 W7</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" xr:uid="{FC9F1E0C-1562-4A4E-84A3-A2B387A65B49}">
+          <x14:formula1>
+            <xm:f>'I:\Y2\Block 3\Project startup\Design Docs\[PeerReview_ArjendeAldrey.xlsx]Data'!#REF!</xm:f>
+          </x14:formula1>
+          <xm:sqref>E10 G10 I10 K10 M10 O10 Q10 S10 U10 W10</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" xr:uid="{0012076C-C599-455C-85C4-6F7216BC973D}">
           <x14:formula1>
             <xm:f>Data!$A$2:$A$9</xm:f>
           </x14:formula1>
-          <xm:sqref>E7:E16 G7:G16 I7:I16 K7:K16 M7:M16 O7:O16 Q7:Q16 S7:S16 U7:U16 W7:W16</xm:sqref>
+          <xm:sqref>I12:I16 K12:K16 M12:M16 O12:O16 Q12:Q16 S12:S16 U12:U16 W12:W16 E12:E16 G12:G16</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -4016,33 +5181,33 @@
         <v>1</v>
       </c>
       <c r="C1" s="2"/>
-      <c r="D1" s="47" t="s">
+      <c r="D1" s="48" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="48"/>
-      <c r="F1" s="48"/>
-      <c r="G1" s="48"/>
-      <c r="H1" s="48"/>
-      <c r="I1" s="48"/>
-      <c r="J1" s="48"/>
-      <c r="K1" s="48"/>
-      <c r="L1" s="48"/>
-      <c r="M1" s="48"/>
-      <c r="N1" s="48"/>
-      <c r="O1" s="48"/>
-      <c r="P1" s="48"/>
-      <c r="Q1" s="48"/>
-      <c r="R1" s="48"/>
-      <c r="S1" s="48"/>
-      <c r="T1" s="48"/>
-      <c r="U1" s="49"/>
-      <c r="V1" s="56" t="s">
+      <c r="E1" s="49"/>
+      <c r="F1" s="49"/>
+      <c r="G1" s="49"/>
+      <c r="H1" s="49"/>
+      <c r="I1" s="49"/>
+      <c r="J1" s="49"/>
+      <c r="K1" s="49"/>
+      <c r="L1" s="49"/>
+      <c r="M1" s="49"/>
+      <c r="N1" s="49"/>
+      <c r="O1" s="49"/>
+      <c r="P1" s="49"/>
+      <c r="Q1" s="49"/>
+      <c r="R1" s="49"/>
+      <c r="S1" s="49"/>
+      <c r="T1" s="49"/>
+      <c r="U1" s="50"/>
+      <c r="V1" s="57" t="s">
         <v>3</v>
       </c>
-      <c r="W1" s="48"/>
-      <c r="X1" s="48"/>
-      <c r="Y1" s="48"/>
-      <c r="Z1" s="48"/>
+      <c r="W1" s="49"/>
+      <c r="X1" s="49"/>
+      <c r="Y1" s="49"/>
+      <c r="Z1" s="49"/>
     </row>
     <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
@@ -4050,31 +5215,31 @@
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="5"/>
-      <c r="D2" s="50" t="s">
+      <c r="D2" s="51" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="51"/>
-      <c r="F2" s="51"/>
-      <c r="G2" s="51"/>
-      <c r="H2" s="51"/>
-      <c r="I2" s="51"/>
-      <c r="J2" s="51"/>
-      <c r="K2" s="51"/>
-      <c r="L2" s="51"/>
-      <c r="M2" s="51"/>
-      <c r="N2" s="51"/>
-      <c r="O2" s="51"/>
-      <c r="P2" s="51"/>
-      <c r="Q2" s="51"/>
-      <c r="R2" s="51"/>
-      <c r="S2" s="51"/>
-      <c r="T2" s="51"/>
-      <c r="U2" s="52"/>
-      <c r="V2" s="57"/>
-      <c r="W2" s="51"/>
-      <c r="X2" s="51"/>
-      <c r="Y2" s="51"/>
-      <c r="Z2" s="51"/>
+      <c r="E2" s="52"/>
+      <c r="F2" s="52"/>
+      <c r="G2" s="52"/>
+      <c r="H2" s="52"/>
+      <c r="I2" s="52"/>
+      <c r="J2" s="52"/>
+      <c r="K2" s="52"/>
+      <c r="L2" s="52"/>
+      <c r="M2" s="52"/>
+      <c r="N2" s="52"/>
+      <c r="O2" s="52"/>
+      <c r="P2" s="52"/>
+      <c r="Q2" s="52"/>
+      <c r="R2" s="52"/>
+      <c r="S2" s="52"/>
+      <c r="T2" s="52"/>
+      <c r="U2" s="53"/>
+      <c r="V2" s="58"/>
+      <c r="W2" s="52"/>
+      <c r="X2" s="52"/>
+      <c r="Y2" s="52"/>
+      <c r="Z2" s="52"/>
     </row>
     <row r="3" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
@@ -4084,31 +5249,31 @@
         <v>7</v>
       </c>
       <c r="C3" s="8"/>
-      <c r="D3" s="53" t="s">
+      <c r="D3" s="54" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="54"/>
-      <c r="F3" s="54"/>
-      <c r="G3" s="54"/>
-      <c r="H3" s="54"/>
-      <c r="I3" s="54"/>
-      <c r="J3" s="54"/>
-      <c r="K3" s="54"/>
-      <c r="L3" s="54"/>
-      <c r="M3" s="54"/>
-      <c r="N3" s="54"/>
-      <c r="O3" s="54"/>
-      <c r="P3" s="54"/>
-      <c r="Q3" s="54"/>
-      <c r="R3" s="54"/>
-      <c r="S3" s="54"/>
-      <c r="T3" s="54"/>
-      <c r="U3" s="55"/>
-      <c r="V3" s="58"/>
-      <c r="W3" s="54"/>
-      <c r="X3" s="54"/>
-      <c r="Y3" s="54"/>
-      <c r="Z3" s="54"/>
+      <c r="E3" s="55"/>
+      <c r="F3" s="55"/>
+      <c r="G3" s="55"/>
+      <c r="H3" s="55"/>
+      <c r="I3" s="55"/>
+      <c r="J3" s="55"/>
+      <c r="K3" s="55"/>
+      <c r="L3" s="55"/>
+      <c r="M3" s="55"/>
+      <c r="N3" s="55"/>
+      <c r="O3" s="55"/>
+      <c r="P3" s="55"/>
+      <c r="Q3" s="55"/>
+      <c r="R3" s="55"/>
+      <c r="S3" s="55"/>
+      <c r="T3" s="55"/>
+      <c r="U3" s="56"/>
+      <c r="V3" s="59"/>
+      <c r="W3" s="55"/>
+      <c r="X3" s="55"/>
+      <c r="Y3" s="55"/>
+      <c r="Z3" s="55"/>
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9"/>
@@ -4176,28 +5341,28 @@
       <c r="A5" s="9"/>
       <c r="B5" s="10"/>
       <c r="C5" s="10"/>
-      <c r="D5" s="63" t="s">
+      <c r="D5" s="64" t="s">
         <v>19</v>
       </c>
-      <c r="E5" s="51"/>
-      <c r="F5" s="51"/>
-      <c r="G5" s="51"/>
-      <c r="H5" s="51"/>
-      <c r="I5" s="51"/>
-      <c r="J5" s="51"/>
-      <c r="K5" s="51"/>
-      <c r="L5" s="51"/>
-      <c r="M5" s="51"/>
-      <c r="N5" s="51"/>
-      <c r="O5" s="51"/>
-      <c r="P5" s="51"/>
-      <c r="Q5" s="51"/>
-      <c r="R5" s="51"/>
-      <c r="S5" s="51"/>
-      <c r="T5" s="51"/>
-      <c r="U5" s="51"/>
-      <c r="V5" s="51"/>
-      <c r="W5" s="51"/>
+      <c r="E5" s="52"/>
+      <c r="F5" s="52"/>
+      <c r="G5" s="52"/>
+      <c r="H5" s="52"/>
+      <c r="I5" s="52"/>
+      <c r="J5" s="52"/>
+      <c r="K5" s="52"/>
+      <c r="L5" s="52"/>
+      <c r="M5" s="52"/>
+      <c r="N5" s="52"/>
+      <c r="O5" s="52"/>
+      <c r="P5" s="52"/>
+      <c r="Q5" s="52"/>
+      <c r="R5" s="52"/>
+      <c r="S5" s="52"/>
+      <c r="T5" s="52"/>
+      <c r="U5" s="52"/>
+      <c r="V5" s="52"/>
+      <c r="W5" s="52"/>
       <c r="X5" s="10"/>
       <c r="Y5" s="16" t="s">
         <v>20</v>
@@ -4291,7 +5456,7 @@
       </c>
     </row>
     <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="62" t="s">
+      <c r="A7" s="63" t="s">
         <v>26</v>
       </c>
       <c r="B7" s="20">
@@ -4345,7 +5510,7 @@
       <c r="Z7" s="27"/>
     </row>
     <row r="8" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="51"/>
+      <c r="A8" s="52"/>
       <c r="B8" s="20">
         <v>12335</v>
       </c>
@@ -4397,7 +5562,7 @@
       <c r="Z8" s="27"/>
     </row>
     <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="51"/>
+      <c r="A9" s="52"/>
       <c r="B9" s="20">
         <v>12335</v>
       </c>
@@ -4449,7 +5614,7 @@
       <c r="Z9" s="27"/>
     </row>
     <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="51"/>
+      <c r="A10" s="52"/>
       <c r="B10" s="20">
         <v>12335</v>
       </c>
@@ -4501,7 +5666,7 @@
       <c r="Z10" s="27"/>
     </row>
     <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="51"/>
+      <c r="A11" s="52"/>
       <c r="B11" s="20">
         <v>12335</v>
       </c>
@@ -4553,7 +5718,7 @@
       <c r="Z11" s="27"/>
     </row>
     <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="51"/>
+      <c r="A12" s="52"/>
       <c r="B12" s="20">
         <v>12335</v>
       </c>
@@ -4605,7 +5770,7 @@
       <c r="Z12" s="27"/>
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="51"/>
+      <c r="A13" s="52"/>
       <c r="B13" s="20">
         <v>12335</v>
       </c>
@@ -4657,7 +5822,7 @@
       <c r="Z13" s="27"/>
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="51"/>
+      <c r="A14" s="52"/>
       <c r="B14" s="20">
         <v>12335</v>
       </c>
@@ -4709,7 +5874,7 @@
       <c r="Z14" s="27"/>
     </row>
     <row r="15" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="51"/>
+      <c r="A15" s="52"/>
       <c r="B15" s="20">
         <v>12335</v>
       </c>
@@ -4761,7 +5926,7 @@
       <c r="Z15" s="27"/>
     </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="51"/>
+      <c r="A16" s="52"/>
       <c r="B16" s="20">
         <v>12335</v>
       </c>
@@ -4891,34 +6056,34 @@
       <c r="Z17" s="32"/>
     </row>
     <row r="18" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="59" t="s">
+      <c r="A18" s="60" t="s">
         <v>40</v>
       </c>
-      <c r="B18" s="60"/>
-      <c r="C18" s="60"/>
-      <c r="D18" s="60"/>
-      <c r="E18" s="60"/>
-      <c r="F18" s="60"/>
-      <c r="G18" s="60"/>
-      <c r="H18" s="60"/>
-      <c r="I18" s="60"/>
-      <c r="J18" s="60"/>
-      <c r="K18" s="60"/>
-      <c r="L18" s="60"/>
-      <c r="M18" s="60"/>
-      <c r="N18" s="60"/>
-      <c r="O18" s="60"/>
-      <c r="P18" s="60"/>
-      <c r="Q18" s="60"/>
-      <c r="R18" s="60"/>
-      <c r="S18" s="60"/>
-      <c r="T18" s="60"/>
-      <c r="U18" s="60"/>
-      <c r="V18" s="60"/>
-      <c r="W18" s="60"/>
-      <c r="X18" s="60"/>
-      <c r="Y18" s="60"/>
-      <c r="Z18" s="61"/>
+      <c r="B18" s="61"/>
+      <c r="C18" s="61"/>
+      <c r="D18" s="61"/>
+      <c r="E18" s="61"/>
+      <c r="F18" s="61"/>
+      <c r="G18" s="61"/>
+      <c r="H18" s="61"/>
+      <c r="I18" s="61"/>
+      <c r="J18" s="61"/>
+      <c r="K18" s="61"/>
+      <c r="L18" s="61"/>
+      <c r="M18" s="61"/>
+      <c r="N18" s="61"/>
+      <c r="O18" s="61"/>
+      <c r="P18" s="61"/>
+      <c r="Q18" s="61"/>
+      <c r="R18" s="61"/>
+      <c r="S18" s="61"/>
+      <c r="T18" s="61"/>
+      <c r="U18" s="61"/>
+      <c r="V18" s="61"/>
+      <c r="W18" s="61"/>
+      <c r="X18" s="61"/>
+      <c r="Y18" s="61"/>
+      <c r="Z18" s="62"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -5023,12 +6188,12 @@
     <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="34"/>
       <c r="B1" s="36" t="str">
-        <f>'Week 2 Review'!C7</f>
+        <f>'Sprint 1'!C7</f>
         <v>Rob O'Connor</v>
       </c>
       <c r="E1" s="34"/>
       <c r="F1" s="36" t="str">
-        <f>'Week 2 Review'!C12</f>
+        <f>'Sprint 1'!C12</f>
         <v>Rowan Ramsey</v>
       </c>
     </row>
@@ -5059,17 +6224,17 @@
         <v>44</v>
       </c>
       <c r="B3" s="39">
-        <f>'Week 2 Review'!E$17</f>
+        <f>'Sprint 1'!E$17</f>
         <v>1</v>
       </c>
       <c r="C3" t="str">
-        <f>'Week 2 Review'!Y$7</f>
+        <f>'Sprint 1'!Y$7</f>
         <v>I planned well for the sprint, good a keeping meetings and
 discussions streamlined, I have a good work ethic and
 can improvise</v>
       </c>
       <c r="D3" t="str">
-        <f>'Week 2 Review'!Z$7</f>
+        <f>'Sprint 1'!Z$7</f>
         <v>I will keep my working hours between 09.30 and 17.00 for 
 most days, I will also try and listen to other peoples ideas 
 a lot better</v>
@@ -5078,15 +6243,15 @@
         <v>44</v>
       </c>
       <c r="F3" s="39">
-        <f>'Week 2 Review'!O$17</f>
+        <f>'Sprint 1'!O$17</f>
         <v>1</v>
       </c>
       <c r="G3">
-        <f>'Week 2 Review'!Y$12</f>
+        <f>'Sprint 1'!Y$12</f>
         <v>0</v>
       </c>
       <c r="H3">
-        <f>'Week 2 Review'!Z$12</f>
+        <f>'Sprint 1'!Z$12</f>
         <v>0</v>
       </c>
     </row>
@@ -5094,32 +6259,32 @@
       <c r="A4" s="34" t="s">
         <v>45</v>
       </c>
-      <c r="B4" s="39" t="str">
-        <f>'Week 4 Review'!E$17</f>
-        <v>NA</v>
-      </c>
-      <c r="C4">
-        <f>'Week 4 Review'!Y$7</f>
-        <v>0</v>
-      </c>
-      <c r="D4">
-        <f>'Week 4 Review'!Z$7</f>
-        <v>0</v>
+      <c r="B4" s="39" t="e">
+        <f>#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="C4" t="e">
+        <f>#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="D4" t="e">
+        <f>#REF!</f>
+        <v>#REF!</v>
       </c>
       <c r="E4" s="34" t="s">
         <v>45</v>
       </c>
-      <c r="F4" s="39" t="str">
-        <f>'Week 4 Review'!O$17</f>
-        <v>NA</v>
-      </c>
-      <c r="G4">
-        <f>'Week 4 Review'!Y$12</f>
-        <v>0</v>
-      </c>
-      <c r="H4">
-        <f>'Week 4 Review'!Z$12</f>
-        <v>0</v>
+      <c r="F4" s="39" t="e">
+        <f>#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="G4" t="e">
+        <f>#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="H4" t="e">
+        <f>#REF!</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5127,42 +6292,42 @@
         <v>46</v>
       </c>
       <c r="B5" s="39" t="str">
-        <f>'Week 6 Review'!E$17</f>
+        <f>'Sprint 3'!E$17</f>
         <v>NA</v>
       </c>
       <c r="C5">
-        <f>'Week 6 Review'!Y$7</f>
+        <f>'Sprint 3'!Y$7</f>
         <v>0</v>
       </c>
       <c r="D5">
-        <f>'Week 6 Review'!Z$7</f>
+        <f>'Sprint 3'!Z$7</f>
         <v>0</v>
       </c>
       <c r="E5" s="34" t="s">
         <v>46</v>
       </c>
       <c r="F5" s="39" t="str">
-        <f>'Week 6 Review'!O$17</f>
+        <f>'Sprint 3'!O$17</f>
         <v>NA</v>
       </c>
       <c r="G5">
-        <f>'Week 6 Review'!Y$12</f>
+        <f>'Sprint 3'!Y$12</f>
         <v>0</v>
       </c>
       <c r="H5">
-        <f>'Week 6 Review'!Z$12</f>
+        <f>'Sprint 3'!Z$12</f>
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="34"/>
       <c r="B6" s="36" t="str">
-        <f>'Week 2 Review'!C8</f>
+        <f>'Sprint 1'!C8</f>
         <v>Tanya Schrijver</v>
       </c>
       <c r="E6" s="34"/>
       <c r="F6" s="36" t="str">
-        <f>'Week 2 Review'!C13</f>
+        <f>'Sprint 1'!C13</f>
         <v>Team Member 7</v>
       </c>
     </row>
@@ -5193,30 +6358,30 @@
         <v>44</v>
       </c>
       <c r="B8" s="39">
-        <f>'Week 2 Review'!G$17</f>
+        <f>'Sprint 1'!G$17</f>
         <v>1</v>
       </c>
-      <c r="C8">
-        <f>'Week 2 Review'!Y$8</f>
-        <v>0</v>
-      </c>
-      <c r="D8">
-        <f>'Week 2 Review'!Z$8</f>
-        <v>0</v>
+      <c r="C8" t="str">
+        <f>'Sprint 1'!Y$8</f>
+        <v>Received very helpful feedback: Be more confident, grant myself more work time and give more feedback to peers.</v>
+      </c>
+      <c r="D8" t="str">
+        <f>'Sprint 1'!Z$8</f>
+        <v>Give myself more work time, keep asking for feedback about my work, give feedback to others more.</v>
       </c>
       <c r="E8" s="34" t="s">
         <v>44</v>
       </c>
       <c r="F8" s="39" t="str">
-        <f>'Week 2 Review'!Q$17</f>
+        <f>'Sprint 1'!Q$17</f>
         <v>NA</v>
       </c>
       <c r="G8">
-        <f>'Week 2 Review'!Y$13</f>
+        <f>'Sprint 1'!Y$13</f>
         <v>0</v>
       </c>
       <c r="H8">
-        <f>'Week 2 Review'!Z$13</f>
+        <f>'Sprint 1'!Z$13</f>
         <v>0</v>
       </c>
     </row>
@@ -5224,32 +6389,32 @@
       <c r="A9" s="34" t="s">
         <v>45</v>
       </c>
-      <c r="B9" s="39" t="str">
-        <f>'Week 4 Review'!G$17</f>
-        <v>NA</v>
-      </c>
-      <c r="C9">
-        <f>'Week 4 Review'!Y$8</f>
-        <v>0</v>
-      </c>
-      <c r="D9">
-        <f>'Week 4 Review'!Z$8</f>
-        <v>0</v>
+      <c r="B9" s="39" t="e">
+        <f>#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="C9" t="e">
+        <f>#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="D9" t="e">
+        <f>#REF!</f>
+        <v>#REF!</v>
       </c>
       <c r="E9" s="34" t="s">
         <v>45</v>
       </c>
-      <c r="F9" s="39" t="str">
-        <f>'Week 4 Review'!Q$17</f>
-        <v>NA</v>
-      </c>
-      <c r="G9">
-        <f>'Week 4 Review'!Y$13</f>
-        <v>0</v>
-      </c>
-      <c r="H9">
-        <f>'Week 4 Review'!Z$13</f>
-        <v>0</v>
+      <c r="F9" s="39" t="e">
+        <f>#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="G9" t="e">
+        <f>#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="H9" t="e">
+        <f>#REF!</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5257,42 +6422,42 @@
         <v>46</v>
       </c>
       <c r="B10" s="39" t="str">
-        <f>'Week 6 Review'!G$17</f>
+        <f>'Sprint 3'!G$17</f>
         <v>NA</v>
       </c>
       <c r="C10">
-        <f>'Week 6 Review'!Y$8</f>
+        <f>'Sprint 3'!Y$8</f>
         <v>0</v>
       </c>
       <c r="D10">
-        <f>'Week 6 Review'!Z$8</f>
+        <f>'Sprint 3'!Z$8</f>
         <v>0</v>
       </c>
       <c r="E10" s="34" t="s">
         <v>46</v>
       </c>
       <c r="F10" s="39" t="str">
-        <f>'Week 6 Review'!Q$17</f>
+        <f>'Sprint 3'!Q$17</f>
         <v>NA</v>
       </c>
       <c r="G10">
-        <f>'Week 6 Review'!Y$13</f>
+        <f>'Sprint 3'!Y$13</f>
         <v>0</v>
       </c>
       <c r="H10">
-        <f>'Week 6 Review'!Z$13</f>
+        <f>'Sprint 3'!Z$13</f>
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="34"/>
       <c r="B11" s="36" t="str">
-        <f>'Week 2 Review'!C9</f>
+        <f>'Sprint 1'!C9</f>
         <v>Humam Abud Allah</v>
       </c>
       <c r="E11" s="34"/>
       <c r="F11" s="36" t="str">
-        <f>'Week 2 Review'!C14</f>
+        <f>'Sprint 1'!C14</f>
         <v>Team Member 8</v>
       </c>
     </row>
@@ -5323,30 +6488,31 @@
         <v>44</v>
       </c>
       <c r="B13" s="39">
-        <f>'Week 2 Review'!I$17</f>
+        <f>'Sprint 1'!I$17</f>
         <v>1</v>
       </c>
-      <c r="C13">
-        <f>'Week 2 Review'!Y$9</f>
-        <v>0</v>
-      </c>
-      <c r="D13">
-        <f>'Week 2 Review'!Z$9</f>
-        <v>0</v>
+      <c r="C13" t="str">
+        <f>'Sprint 1'!Y$9</f>
+        <v xml:space="preserve">As a summary, according to my team mates I always deliever what's asked from me in high quality and can be relied on even in areas that are not my expertise. I always ask for feedback, even during the process.
+</v>
+      </c>
+      <c r="D13" t="str">
+        <f>'Sprint 1'!Z$9</f>
+        <v>For improvments I need to be more communicative with my team mates during work, meaning less time on headphones and more time being present.</v>
       </c>
       <c r="E13" s="34" t="s">
         <v>44</v>
       </c>
       <c r="F13" s="39" t="str">
-        <f>'Week 2 Review'!S$17</f>
+        <f>'Sprint 1'!S$17</f>
         <v>NA</v>
       </c>
       <c r="G13">
-        <f>'Week 2 Review'!Y$14</f>
+        <f>'Sprint 1'!Y$14</f>
         <v>0</v>
       </c>
       <c r="H13">
-        <f>'Week 2 Review'!Z$14</f>
+        <f>'Sprint 1'!Z$14</f>
         <v>0</v>
       </c>
     </row>
@@ -5354,32 +6520,32 @@
       <c r="A14" s="34" t="s">
         <v>45</v>
       </c>
-      <c r="B14" s="39" t="str">
-        <f>'Week 4 Review'!I$17</f>
-        <v>NA</v>
-      </c>
-      <c r="C14">
-        <f>'Week 4 Review'!Y$9</f>
-        <v>0</v>
-      </c>
-      <c r="D14">
-        <f>'Week 4 Review'!Z$9</f>
-        <v>0</v>
+      <c r="B14" s="39" t="e">
+        <f>#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="C14" t="e">
+        <f>#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="D14" t="e">
+        <f>#REF!</f>
+        <v>#REF!</v>
       </c>
       <c r="E14" s="34" t="s">
         <v>45</v>
       </c>
-      <c r="F14" s="39" t="str">
-        <f>'Week 4 Review'!S$17</f>
-        <v>NA</v>
-      </c>
-      <c r="G14">
-        <f>'Week 4 Review'!Y$14</f>
-        <v>0</v>
-      </c>
-      <c r="H14">
-        <f>'Week 4 Review'!Z$14</f>
-        <v>0</v>
+      <c r="F14" s="39" t="e">
+        <f>#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="G14" t="e">
+        <f>#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="H14" t="e">
+        <f>#REF!</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5387,42 +6553,42 @@
         <v>46</v>
       </c>
       <c r="B15" s="39" t="str">
-        <f>'Week 6 Review'!I$17</f>
+        <f>'Sprint 3'!I$17</f>
         <v>NA</v>
       </c>
       <c r="C15">
-        <f>'Week 6 Review'!Y$9</f>
+        <f>'Sprint 3'!Y$9</f>
         <v>0</v>
       </c>
       <c r="D15">
-        <f>'Week 6 Review'!Z$9</f>
+        <f>'Sprint 3'!Z$9</f>
         <v>0</v>
       </c>
       <c r="E15" s="34" t="s">
         <v>46</v>
       </c>
       <c r="F15" s="39" t="str">
-        <f>'Week 6 Review'!S$17</f>
+        <f>'Sprint 3'!S$17</f>
         <v>NA</v>
       </c>
       <c r="G15">
-        <f>'Week 6 Review'!Y$14</f>
+        <f>'Sprint 3'!Y$14</f>
         <v>0</v>
       </c>
       <c r="H15">
-        <f>'Week 6 Review'!Z$14</f>
+        <f>'Sprint 3'!Z$14</f>
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="34"/>
       <c r="B16" s="36" t="str">
-        <f>'Week 2 Review'!C10</f>
+        <f>'Sprint 1'!C10</f>
         <v>Arjen de Aldrey</v>
       </c>
       <c r="E16" s="34"/>
       <c r="F16" s="36" t="str">
-        <f>'Week 2 Review'!C15</f>
+        <f>'Sprint 1'!C15</f>
         <v>Team Member 9</v>
       </c>
       <c r="H16" s="34"/>
@@ -5454,30 +6620,30 @@
         <v>44</v>
       </c>
       <c r="B18" s="39">
-        <f>'Week 2 Review'!K$17</f>
+        <f>'Sprint 1'!K$17</f>
         <v>1</v>
       </c>
-      <c r="C18">
-        <f>'Week 2 Review'!Y$10</f>
-        <v>0</v>
-      </c>
-      <c r="D18">
-        <f>'Week 2 Review'!Z$10</f>
-        <v>0</v>
+      <c r="C18" t="str">
+        <f>'Sprint 1'!Y$10</f>
+        <v>Quick at making prototypes and isn't afraid to add or remove features when asked. Gets distracted sometimes. Gives advice but sometimes get stuck on specific points. Learn more about advanced c++ concepts and ask sooner for help.</v>
+      </c>
+      <c r="D18" t="str">
+        <f>'Sprint 1'!Z$10</f>
+        <v>Dabble with more C++ in general but more specifically advanced data structures. Make decisions more quickly instead of arguing about it.</v>
       </c>
       <c r="E18" s="34" t="s">
         <v>44</v>
       </c>
       <c r="F18" s="39" t="str">
-        <f>'Week 2 Review'!U$17</f>
+        <f>'Sprint 1'!U$17</f>
         <v>NA</v>
       </c>
       <c r="G18">
-        <f>'Week 2 Review'!Y$15</f>
+        <f>'Sprint 1'!Y$15</f>
         <v>0</v>
       </c>
       <c r="H18">
-        <f>'Week 2 Review'!Z$15</f>
+        <f>'Sprint 1'!Z$15</f>
         <v>0</v>
       </c>
     </row>
@@ -5485,32 +6651,32 @@
       <c r="A19" s="34" t="s">
         <v>45</v>
       </c>
-      <c r="B19" s="39" t="str">
-        <f>'Week 4 Review'!K$17</f>
-        <v>NA</v>
-      </c>
-      <c r="C19">
-        <f>'Week 4 Review'!Y$10</f>
-        <v>0</v>
-      </c>
-      <c r="D19">
-        <f>'Week 4 Review'!Z$10</f>
-        <v>0</v>
+      <c r="B19" s="39" t="e">
+        <f>#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="C19" t="e">
+        <f>#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="D19" t="e">
+        <f>#REF!</f>
+        <v>#REF!</v>
       </c>
       <c r="E19" s="34" t="s">
         <v>45</v>
       </c>
-      <c r="F19" s="39" t="str">
-        <f>'Week 4 Review'!U$17</f>
-        <v>NA</v>
-      </c>
-      <c r="G19">
-        <f>'Week 4 Review'!Y$15</f>
-        <v>0</v>
-      </c>
-      <c r="H19">
-        <f>'Week 4 Review'!Z$15</f>
-        <v>0</v>
+      <c r="F19" s="39" t="e">
+        <f>#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="G19" t="e">
+        <f>#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="H19" t="e">
+        <f>#REF!</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5518,42 +6684,42 @@
         <v>46</v>
       </c>
       <c r="B20" s="39" t="str">
-        <f>'Week 6 Review'!K$17</f>
+        <f>'Sprint 3'!K$17</f>
         <v>NA</v>
       </c>
       <c r="C20">
-        <f>'Week 6 Review'!Y$10</f>
+        <f>'Sprint 3'!Y$10</f>
         <v>0</v>
       </c>
       <c r="D20">
-        <f>'Week 6 Review'!Z$10</f>
+        <f>'Sprint 3'!Z$10</f>
         <v>0</v>
       </c>
       <c r="E20" s="34" t="s">
         <v>46</v>
       </c>
       <c r="F20" s="39" t="str">
-        <f>'Week 6 Review'!U$17</f>
+        <f>'Sprint 3'!U$17</f>
         <v>NA</v>
       </c>
       <c r="G20">
-        <f>'Week 6 Review'!Y$15</f>
+        <f>'Sprint 3'!Y$15</f>
         <v>0</v>
       </c>
       <c r="H20">
-        <f>'Week 6 Review'!Z$15</f>
+        <f>'Sprint 3'!Z$15</f>
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="34"/>
       <c r="B21" s="36" t="str">
-        <f>'Week 2 Review'!C11</f>
+        <f>'Sprint 1'!C11</f>
         <v>Glyn Leine</v>
       </c>
       <c r="E21" s="34"/>
       <c r="F21" s="36" t="str">
-        <f>'Week 2 Review'!C16</f>
+        <f>'Sprint 1'!C16</f>
         <v>Team Member 10</v>
       </c>
       <c r="G21" s="34"/>
@@ -5586,30 +6752,30 @@
         <v>44</v>
       </c>
       <c r="B23" s="39">
-        <f>'Week 2 Review'!M$17</f>
+        <f>'Sprint 1'!M$17</f>
         <v>1</v>
       </c>
-      <c r="C23">
-        <f>'Week 2 Review'!Y$11</f>
-        <v>0</v>
-      </c>
-      <c r="D23">
-        <f>'Week 2 Review'!Z$11</f>
-        <v>0</v>
+      <c r="C23" t="str">
+        <f>'Sprint 1'!Y$11</f>
+        <v>I keep getting stuck on no longer relevant topics during discussions, dragging out discussions unnecessarily. Should learn better time management.</v>
+      </c>
+      <c r="D23" t="str">
+        <f>'Sprint 1'!Z$11</f>
+        <v>I should rethink whether what I want to say is really still relevant. I should trust my fellow programmers with bigger tasks and add an even higher time margin to tasks.</v>
       </c>
       <c r="E23" s="34" t="s">
         <v>44</v>
       </c>
       <c r="F23" s="39" t="str">
-        <f>'Week 2 Review'!W$17</f>
+        <f>'Sprint 1'!W$17</f>
         <v>NA</v>
       </c>
       <c r="G23">
-        <f>'Week 2 Review'!Y$16</f>
+        <f>'Sprint 1'!Y$16</f>
         <v>0</v>
       </c>
       <c r="H23">
-        <f>'Week 2 Review'!Z$16</f>
+        <f>'Sprint 1'!Z$16</f>
         <v>0</v>
       </c>
     </row>
@@ -5617,32 +6783,32 @@
       <c r="A24" s="34" t="s">
         <v>45</v>
       </c>
-      <c r="B24" s="39" t="str">
-        <f>'Week 4 Review'!M$17</f>
-        <v>NA</v>
-      </c>
-      <c r="C24">
-        <f>'Week 4 Review'!Y$11</f>
-        <v>0</v>
-      </c>
-      <c r="D24">
-        <f>'Week 4 Review'!Z$11</f>
-        <v>0</v>
+      <c r="B24" s="39" t="e">
+        <f>#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="C24" t="e">
+        <f>#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="D24" t="e">
+        <f>#REF!</f>
+        <v>#REF!</v>
       </c>
       <c r="E24" s="34" t="s">
         <v>45</v>
       </c>
-      <c r="F24" s="39" t="str">
-        <f>'Week 4 Review'!W$17</f>
-        <v>NA</v>
-      </c>
-      <c r="G24">
-        <f>'Week 4 Review'!Y$16</f>
-        <v>0</v>
-      </c>
-      <c r="H24">
-        <f>'Week 4 Review'!Z$16</f>
-        <v>0</v>
+      <c r="F24" s="39" t="e">
+        <f>#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="G24" t="e">
+        <f>#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="H24" t="e">
+        <f>#REF!</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5650,30 +6816,30 @@
         <v>46</v>
       </c>
       <c r="B25" s="39" t="str">
-        <f>'Week 6 Review'!M$17</f>
+        <f>'Sprint 3'!M$17</f>
         <v>NA</v>
       </c>
       <c r="C25">
-        <f>'Week 6 Review'!Y$11</f>
+        <f>'Sprint 3'!Y$11</f>
         <v>0</v>
       </c>
       <c r="D25">
-        <f>'Week 6 Review'!Z$11</f>
+        <f>'Sprint 3'!Z$11</f>
         <v>0</v>
       </c>
       <c r="E25" s="34" t="s">
         <v>46</v>
       </c>
       <c r="F25" s="39" t="str">
-        <f>'Week 6 Review'!W$17</f>
+        <f>'Sprint 3'!W$17</f>
         <v>NA</v>
       </c>
       <c r="G25">
-        <f>'Week 6 Review'!Y$16</f>
+        <f>'Sprint 3'!Y$16</f>
         <v>0</v>
       </c>
       <c r="H25">
-        <f>'Week 6 Review'!Z$16</f>
+        <f>'Sprint 3'!Z$16</f>
         <v>0</v>
       </c>
     </row>

</xml_diff>